<commit_message>
Adding functions and solving bugs in KMO
</commit_message>
<xml_diff>
--- a/data/Dataset_2/reduced_dataframe_FA2.xlsx
+++ b/data/Dataset_2/reduced_dataframe_FA2.xlsx
@@ -451,12 +451,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>spectral_flatness</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>DeltaFreq</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -479,10 +479,10 @@
         <v>0.03291599999999996</v>
       </c>
       <c r="E2" t="n">
+        <v>0.4643990929705216</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.4455689787864685</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4198.974609375</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -504,10 +504,10 @@
         <v>0.5895352</v>
       </c>
       <c r="E3" t="n">
+        <v>2.159455782312925</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.4866604804992676</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2347.119140625</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -529,10 +529,10 @@
         <v>-0.9326319999999999</v>
       </c>
       <c r="E4" t="n">
+        <v>3.842902494331066</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.6496953368186951</v>
-      </c>
-      <c r="F4" t="n">
-        <v>279.931640625</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -554,10 +554,10 @@
         <v>-0.1298318</v>
       </c>
       <c r="E5" t="n">
+        <v>6.838276643990929</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.4340538680553436</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2433.251953125</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -579,10 +579,10 @@
         <v>-0.3966268</v>
       </c>
       <c r="E6" t="n">
+        <v>7.37233560090703</v>
+      </c>
+      <c r="F6" t="n">
         <v>0.411316841840744</v>
-      </c>
-      <c r="F6" t="n">
-        <v>366.064453125</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -604,10 +604,10 @@
         <v>-0.3446670000000001</v>
       </c>
       <c r="E7" t="n">
+        <v>8.126984126984127</v>
+      </c>
+      <c r="F7" t="n">
         <v>0.2180296778678894</v>
-      </c>
-      <c r="F7" t="n">
-        <v>430.6640625</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -629,10 +629,10 @@
         <v>-0.07355299999999999</v>
       </c>
       <c r="E8" t="n">
+        <v>8.568163265306122</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.3577386438846588</v>
-      </c>
-      <c r="F8" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -654,10 +654,10 @@
         <v>0.157636</v>
       </c>
       <c r="E9" t="n">
+        <v>9.287981859410431</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.2040617913007736</v>
-      </c>
-      <c r="F9" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -679,10 +679,10 @@
         <v>0.873655</v>
       </c>
       <c r="E10" t="n">
+        <v>10.43736961451247</v>
+      </c>
+      <c r="F10" t="n">
         <v>0.2519037127494812</v>
-      </c>
-      <c r="F10" t="n">
-        <v>602.9296875</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -704,10 +704,10 @@
         <v>0.02676400000000001</v>
       </c>
       <c r="E11" t="n">
+        <v>10.95981859410431</v>
+      </c>
+      <c r="F11" t="n">
         <v>0.2411715388298035</v>
-      </c>
-      <c r="F11" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -729,10 +729,10 @@
         <v>0.579855</v>
       </c>
       <c r="E12" t="n">
+        <v>11.45904761904762</v>
+      </c>
+      <c r="F12" t="n">
         <v>0.3559316992759705</v>
-      </c>
-      <c r="F12" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -754,10 +754,10 @@
         <v>0.06209495</v>
       </c>
       <c r="E13" t="n">
+        <v>11.96988662131519</v>
+      </c>
+      <c r="F13" t="n">
         <v>0.3428803384304047</v>
-      </c>
-      <c r="F13" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -779,10 +779,10 @@
         <v>-0.07375799999999999</v>
       </c>
       <c r="E14" t="n">
+        <v>12.44589569160998</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.2459251433610916</v>
-      </c>
-      <c r="F14" t="n">
-        <v>624.462890625</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -804,10 +804,10 @@
         <v>-0.470606</v>
       </c>
       <c r="E15" t="n">
+        <v>12.92190476190476</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.2714539766311646</v>
-      </c>
-      <c r="F15" t="n">
-        <v>624.462890625</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -829,10 +829,10 @@
         <v>-0.02568939999999999</v>
       </c>
       <c r="E16" t="n">
+        <v>13.4443537414966</v>
+      </c>
+      <c r="F16" t="n">
         <v>0.4103755354881287</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2239.453125</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -854,10 +854,10 @@
         <v>0.9919790000000001</v>
       </c>
       <c r="E17" t="n">
+        <v>14.43120181405896</v>
+      </c>
+      <c r="F17" t="n">
         <v>0.2984591722488403</v>
-      </c>
-      <c r="F17" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -879,10 +879,10 @@
         <v>0.1674006</v>
       </c>
       <c r="E18" t="n">
+        <v>14.81433106575964</v>
+      </c>
+      <c r="F18" t="n">
         <v>0.2929583489894867</v>
-      </c>
-      <c r="F18" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -904,10 +904,10 @@
         <v>0.459443</v>
       </c>
       <c r="E19" t="n">
+        <v>15.41804988662131</v>
+      </c>
+      <c r="F19" t="n">
         <v>0.2419058233499527</v>
-      </c>
-      <c r="F19" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -929,10 +929,10 @@
         <v>0.504266</v>
       </c>
       <c r="E20" t="n">
+        <v>15.88244897959184</v>
+      </c>
+      <c r="F20" t="n">
         <v>0.2620352208614349</v>
-      </c>
-      <c r="F20" t="n">
-        <v>645.99609375</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -954,10 +954,10 @@
         <v>1.00679</v>
       </c>
       <c r="E21" t="n">
+        <v>16.34684807256236</v>
+      </c>
+      <c r="F21" t="n">
         <v>0.2289713472127914</v>
-      </c>
-      <c r="F21" t="n">
-        <v>645.99609375</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -979,10 +979,10 @@
         <v>-0.3869669999999999</v>
       </c>
       <c r="E22" t="n">
+        <v>16.57904761904762</v>
+      </c>
+      <c r="F22" t="n">
         <v>0.6758666634559631</v>
-      </c>
-      <c r="F22" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1004,10 +1004,10 @@
         <v>-1.409166</v>
       </c>
       <c r="E23" t="n">
+        <v>16.76480725623583</v>
+      </c>
+      <c r="F23" t="n">
         <v>0.2705444395542145</v>
-      </c>
-      <c r="F23" t="n">
-        <v>689.0625</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1029,10 +1029,10 @@
         <v>0.258779</v>
       </c>
       <c r="E24" t="n">
+        <v>17.79809523809524</v>
+      </c>
+      <c r="F24" t="n">
         <v>0.2253943234682083</v>
-      </c>
-      <c r="F24" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1054,10 +1054,10 @@
         <v>0.216231</v>
       </c>
       <c r="E25" t="n">
+        <v>18.27410430839002</v>
+      </c>
+      <c r="F25" t="n">
         <v>0.2520084977149963</v>
-      </c>
-      <c r="F25" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1079,10 +1079,10 @@
         <v>0.2697415</v>
       </c>
       <c r="E26" t="n">
+        <v>18.76172335600907</v>
+      </c>
+      <c r="F26" t="n">
         <v>0.3615876138210297</v>
-      </c>
-      <c r="F26" t="n">
-        <v>624.462890625</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         <v>0.8828710000000001</v>
       </c>
       <c r="E27" t="n">
+        <v>19.26095238095238</v>
+      </c>
+      <c r="F27" t="n">
         <v>0.3528262376785278</v>
-      </c>
-      <c r="F27" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1129,10 +1129,10 @@
         <v>0.482227</v>
       </c>
       <c r="E28" t="n">
+        <v>19.74857142857143</v>
+      </c>
+      <c r="F28" t="n">
         <v>0.2835486829280853</v>
-      </c>
-      <c r="F28" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1154,10 +1154,10 @@
         <v>0.095638</v>
       </c>
       <c r="E29" t="n">
+        <v>20.14331065759637</v>
+      </c>
+      <c r="F29" t="n">
         <v>0.3418993353843689</v>
-      </c>
-      <c r="F29" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1179,10 +1179,10 @@
         <v>0.61032</v>
       </c>
       <c r="E30" t="n">
+        <v>20.71219954648526</v>
+      </c>
+      <c r="F30" t="n">
         <v>0.267776221036911</v>
-      </c>
-      <c r="F30" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1204,10 +1204,10 @@
         <v>-0.009956700000000004</v>
       </c>
       <c r="E31" t="n">
+        <v>21.2346485260771</v>
+      </c>
+      <c r="F31" t="n">
         <v>0.3027820587158203</v>
-      </c>
-      <c r="F31" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1229,10 +1229,10 @@
         <v>0.8685700000000001</v>
       </c>
       <c r="E32" t="n">
+        <v>21.73387755102041</v>
+      </c>
+      <c r="F32" t="n">
         <v>0.2617036700248718</v>
-      </c>
-      <c r="F32" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1254,10 +1254,10 @@
         <v>-0.2709188</v>
       </c>
       <c r="E33" t="n">
+        <v>22.19827664399093</v>
+      </c>
+      <c r="F33" t="n">
         <v>0.3808356523513794</v>
-      </c>
-      <c r="F33" t="n">
-        <v>3552.978515625</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1279,10 +1279,10 @@
         <v>0.5736519999999999</v>
       </c>
       <c r="E34" t="n">
+        <v>22.88326530612245</v>
+      </c>
+      <c r="F34" t="n">
         <v>0.2450205087661743</v>
-      </c>
-      <c r="F34" t="n">
-        <v>882.861328125</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1304,10 +1304,10 @@
         <v>-0.2520979999999999</v>
       </c>
       <c r="E35" t="n">
+        <v>23.88172335600907</v>
+      </c>
+      <c r="F35" t="n">
         <v>0.3084115087985992</v>
-      </c>
-      <c r="F35" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1329,10 +1329,10 @@
         <v>0.28705</v>
       </c>
       <c r="E36" t="n">
+        <v>24.40417233560091</v>
+      </c>
+      <c r="F36" t="n">
         <v>0.2630535960197449</v>
-      </c>
-      <c r="F36" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1354,10 +1354,10 @@
         <v>0.102025</v>
       </c>
       <c r="E37" t="n">
+        <v>24.8453514739229</v>
+      </c>
+      <c r="F37" t="n">
         <v>0.43234983086586</v>
-      </c>
-      <c r="F37" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1379,10 +1379,10 @@
         <v>-0.972083</v>
       </c>
       <c r="E38" t="n">
+        <v>25.43746031746032</v>
+      </c>
+      <c r="F38" t="n">
         <v>0.2850871384143829</v>
-      </c>
-      <c r="F38" t="n">
-        <v>645.99609375</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1404,10 +1404,10 @@
         <v>-0.44925048</v>
       </c>
       <c r="E39" t="n">
+        <v>27.10929705215419</v>
+      </c>
+      <c r="F39" t="n">
         <v>0.3371286392211914</v>
-      </c>
-      <c r="F39" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>-0.18190752</v>
       </c>
       <c r="E40" t="n">
+        <v>27.66657596371882</v>
+      </c>
+      <c r="F40" t="n">
         <v>0.2582423388957977</v>
-      </c>
-      <c r="F40" t="n">
-        <v>667.529296875</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1454,10 +1454,10 @@
         <v>-0.1621885</v>
       </c>
       <c r="E41" t="n">
+        <v>28.22385487528345</v>
+      </c>
+      <c r="F41" t="n">
         <v>0.3662774860858917</v>
-      </c>
-      <c r="F41" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1479,10 +1479,10 @@
         <v>-0.6010150000000001</v>
       </c>
       <c r="E42" t="n">
+        <v>28.75791383219955</v>
+      </c>
+      <c r="F42" t="n">
         <v>0.3465336263179779</v>
-      </c>
-      <c r="F42" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1504,10 +1504,10 @@
         <v>0.1545904</v>
       </c>
       <c r="E43" t="n">
+        <v>29.76798185941043</v>
+      </c>
+      <c r="F43" t="n">
         <v>0.2540142238140106</v>
-      </c>
-      <c r="F43" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1529,10 +1529,10 @@
         <v>-0.5531848</v>
       </c>
       <c r="E44" t="n">
+        <v>30.31365079365079</v>
+      </c>
+      <c r="F44" t="n">
         <v>0.3672841787338257</v>
-      </c>
-      <c r="F44" t="n">
-        <v>645.99609375</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1554,10 +1554,10 @@
         <v>0.315715</v>
       </c>
       <c r="E45" t="n">
+        <v>30.85931972789116</v>
+      </c>
+      <c r="F45" t="n">
         <v>0.2683643102645874</v>
-      </c>
-      <c r="F45" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1579,10 +1579,10 @@
         <v>-0.32358</v>
       </c>
       <c r="E46" t="n">
+        <v>31.40498866213152</v>
+      </c>
+      <c r="F46" t="n">
         <v>0.2652334570884705</v>
-      </c>
-      <c r="F46" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1604,10 +1604,10 @@
         <v>0.253869</v>
       </c>
       <c r="E47" t="n">
+        <v>31.90421768707483</v>
+      </c>
+      <c r="F47" t="n">
         <v>0.2661702334880829</v>
-      </c>
-      <c r="F47" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1629,10 +1629,10 @@
         <v>0.09864700000000001</v>
       </c>
       <c r="E48" t="n">
+        <v>32.51954648526077</v>
+      </c>
+      <c r="F48" t="n">
         <v>0.2279416918754578</v>
-      </c>
-      <c r="F48" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -1654,10 +1654,10 @@
         <v>-0.3814044</v>
       </c>
       <c r="E49" t="n">
+        <v>34.42358276643991</v>
+      </c>
+      <c r="F49" t="n">
         <v>0.3464130163192749</v>
-      </c>
-      <c r="F49" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -1679,10 +1679,10 @@
         <v>-0.5612010000000001</v>
       </c>
       <c r="E50" t="n">
+        <v>34.92281179138322</v>
+      </c>
+      <c r="F50" t="n">
         <v>0.2848648130893707</v>
-      </c>
-      <c r="F50" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -1704,10 +1704,10 @@
         <v>0.3299030000000001</v>
       </c>
       <c r="E51" t="n">
+        <v>35.70068027210884</v>
+      </c>
+      <c r="F51" t="n">
         <v>0.3439965844154358</v>
-      </c>
-      <c r="F51" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -1729,10 +1729,10 @@
         <v>-0.522292</v>
       </c>
       <c r="E52" t="n">
+        <v>36.25795918367347</v>
+      </c>
+      <c r="F52" t="n">
         <v>0.3653849959373474</v>
-      </c>
-      <c r="F52" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -1754,10 +1754,10 @@
         <v>-0.004835999999999993</v>
       </c>
       <c r="E53" t="n">
+        <v>36.78040816326531</v>
+      </c>
+      <c r="F53" t="n">
         <v>0.3609646558761597</v>
-      </c>
-      <c r="F53" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -1779,10 +1779,10 @@
         <v>-0.2995420000000001</v>
       </c>
       <c r="E54" t="n">
+        <v>37.65115646258504</v>
+      </c>
+      <c r="F54" t="n">
         <v>0.3714932203292847</v>
-      </c>
-      <c r="F54" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -1804,10 +1804,10 @@
         <v>-0.004326000000000002</v>
       </c>
       <c r="E55" t="n">
+        <v>38.12716553287982</v>
+      </c>
+      <c r="F55" t="n">
         <v>0.3863250315189362</v>
-      </c>
-      <c r="F55" t="n">
-        <v>2497.8515625</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -1829,10 +1829,10 @@
         <v>0.473526</v>
       </c>
       <c r="E56" t="n">
+        <v>38.56834467120181</v>
+      </c>
+      <c r="F56" t="n">
         <v>0.3241146206855774</v>
-      </c>
-      <c r="F56" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -1854,10 +1854,10 @@
         <v>-0.5135358000000001</v>
       </c>
       <c r="E57" t="n">
+        <v>39.0443537414966</v>
+      </c>
+      <c r="F57" t="n">
         <v>0.3618713319301605</v>
-      </c>
-      <c r="F57" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -1879,10 +1879,10 @@
         <v>-0.1989396</v>
       </c>
       <c r="E58" t="n">
+        <v>39.50875283446712</v>
+      </c>
+      <c r="F58" t="n">
         <v>0.3444554805755615</v>
-      </c>
-      <c r="F58" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -1904,10 +1904,10 @@
         <v>0.261233</v>
       </c>
       <c r="E59" t="n">
+        <v>40.03120181405896</v>
+      </c>
+      <c r="F59" t="n">
         <v>0.3196444511413574</v>
-      </c>
-      <c r="F59" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -1929,10 +1929,10 @@
         <v>0.224087</v>
       </c>
       <c r="E60" t="n">
+        <v>40.47238095238095</v>
+      </c>
+      <c r="F60" t="n">
         <v>0.3192424774169922</v>
-      </c>
-      <c r="F60" t="n">
-        <v>861.328125</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -1954,10 +1954,10 @@
         <v>-0.262425</v>
       </c>
       <c r="E61" t="n">
+        <v>40.93678004535148</v>
+      </c>
+      <c r="F61" t="n">
         <v>0.3505704402923584</v>
-      </c>
-      <c r="F61" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -1979,10 +1979,10 @@
         <v>-0.05543159999999997</v>
       </c>
       <c r="E62" t="n">
+        <v>41.4940589569161</v>
+      </c>
+      <c r="F62" t="n">
         <v>0.3298690915107727</v>
-      </c>
-      <c r="F62" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2004,10 +2004,10 @@
         <v>-0.1707904</v>
       </c>
       <c r="E63" t="n">
+        <v>42.37641723356009</v>
+      </c>
+      <c r="F63" t="n">
         <v>0.4078971743583679</v>
-      </c>
-      <c r="F63" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2029,10 +2029,10 @@
         <v>0.2262165</v>
       </c>
       <c r="E64" t="n">
+        <v>42.82920634920635</v>
+      </c>
+      <c r="F64" t="n">
         <v>0.3345603346824646</v>
-      </c>
-      <c r="F64" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         <v>0.340125</v>
       </c>
       <c r="E65" t="n">
+        <v>43.29360544217687</v>
+      </c>
+      <c r="F65" t="n">
         <v>0.3361167907714844</v>
-      </c>
-      <c r="F65" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2079,10 +2079,10 @@
         <v>-0.175461</v>
       </c>
       <c r="E66" t="n">
+        <v>43.8160544217687</v>
+      </c>
+      <c r="F66" t="n">
         <v>0.3619206845760345</v>
-      </c>
-      <c r="F66" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2104,10 +2104,10 @@
         <v>0.417245</v>
       </c>
       <c r="E67" t="n">
+        <v>44.31528344671202</v>
+      </c>
+      <c r="F67" t="n">
         <v>0.3660061955451965</v>
-      </c>
-      <c r="F67" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2129,10 +2129,10 @@
         <v>0.02845600000000001</v>
       </c>
       <c r="E68" t="n">
+        <v>44.44299319727891</v>
+      </c>
+      <c r="F68" t="n">
         <v>0.4930038452148438</v>
-      </c>
-      <c r="F68" t="n">
-        <v>2476.318359375</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>0.462775</v>
       </c>
       <c r="E69" t="n">
+        <v>45.29052154195011</v>
+      </c>
+      <c r="F69" t="n">
         <v>0.3066600859165192</v>
-      </c>
-      <c r="F69" t="n">
-        <v>2476.318359375</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2179,10 +2179,10 @@
         <v>-0.125634</v>
       </c>
       <c r="E70" t="n">
+        <v>46.27736961451247</v>
+      </c>
+      <c r="F70" t="n">
         <v>0.3166759610176086</v>
-      </c>
-      <c r="F70" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2204,10 +2204,10 @@
         <v>0.190708</v>
       </c>
       <c r="E71" t="n">
+        <v>46.7069387755102</v>
+      </c>
+      <c r="F71" t="n">
         <v>0.3761717081069946</v>
-      </c>
-      <c r="F71" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2229,10 +2229,10 @@
         <v>-0.361339</v>
       </c>
       <c r="E72" t="n">
+        <v>47.42675736961451</v>
+      </c>
+      <c r="F72" t="n">
         <v>0.3909133672714233</v>
-      </c>
-      <c r="F72" t="n">
-        <v>2497.8515625</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         <v>0.0408183</v>
       </c>
       <c r="E73" t="n">
+        <v>48.55292517006803</v>
+      </c>
+      <c r="F73" t="n">
         <v>0.3823809027671814</v>
-      </c>
-      <c r="F73" t="n">
-        <v>2368.65234375</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2279,10 +2279,10 @@
         <v>-0.5896520000000001</v>
       </c>
       <c r="E74" t="n">
+        <v>49.04054421768708</v>
+      </c>
+      <c r="F74" t="n">
         <v>0.3574503064155579</v>
-      </c>
-      <c r="F74" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2304,10 +2304,10 @@
         <v>-1.198194</v>
       </c>
       <c r="E75" t="n">
+        <v>49.50494331065759</v>
+      </c>
+      <c r="F75" t="n">
         <v>0.3574751615524292</v>
-      </c>
-      <c r="F75" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2329,10 +2329,10 @@
         <v>-1.268632</v>
       </c>
       <c r="E76" t="n">
+        <v>49.95773242630386</v>
+      </c>
+      <c r="F76" t="n">
         <v>0.3723783493041992</v>
-      </c>
-      <c r="F76" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2354,10 +2354,10 @@
         <v>0.647303</v>
       </c>
       <c r="E77" t="n">
+        <v>50.45696145124717</v>
+      </c>
+      <c r="F77" t="n">
         <v>0.3463893234729767</v>
-      </c>
-      <c r="F77" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2379,10 +2379,10 @@
         <v>0.139216</v>
       </c>
       <c r="E78" t="n">
+        <v>50.89814058956916</v>
+      </c>
+      <c r="F78" t="n">
         <v>0.3581941723823547</v>
-      </c>
-      <c r="F78" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2404,10 +2404,10 @@
         <v>-0.0625776</v>
       </c>
       <c r="E79" t="n">
+        <v>52.19845804988662</v>
+      </c>
+      <c r="F79" t="n">
         <v>0.2964995205402374</v>
-      </c>
-      <c r="F79" t="n">
-        <v>2217.919921875</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2429,10 +2429,10 @@
         <v>0.005269400000000001</v>
       </c>
       <c r="E80" t="n">
+        <v>53.1156462585034</v>
+      </c>
+      <c r="F80" t="n">
         <v>0.3248679637908936</v>
-      </c>
-      <c r="F80" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2454,10 +2454,10 @@
         <v>-0.462176</v>
       </c>
       <c r="E81" t="n">
+        <v>53.5568253968254</v>
+      </c>
+      <c r="F81" t="n">
         <v>0.3710368573665619</v>
-      </c>
-      <c r="F81" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -2479,10 +2479,10 @@
         <v>0.2689708</v>
       </c>
       <c r="E82" t="n">
+        <v>55.83238095238095</v>
+      </c>
+      <c r="F82" t="n">
         <v>0.3768153190612793</v>
-      </c>
-      <c r="F82" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -2504,10 +2504,10 @@
         <v>-0.8353780000000001</v>
       </c>
       <c r="E83" t="n">
+        <v>56.28517006802721</v>
+      </c>
+      <c r="F83" t="n">
         <v>0.3444229364395142</v>
-      </c>
-      <c r="F83" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -2529,10 +2529,10 @@
         <v>-0.475745</v>
       </c>
       <c r="E84" t="n">
+        <v>56.73795918367347</v>
+      </c>
+      <c r="F84" t="n">
         <v>0.3310630619525909</v>
-      </c>
-      <c r="F84" t="n">
-        <v>2260.986328125</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -2554,10 +2554,10 @@
         <v>0.3791252</v>
       </c>
       <c r="E85" t="n">
+        <v>57.63192743764172</v>
+      </c>
+      <c r="F85" t="n">
         <v>0.3465378880500793</v>
-      </c>
-      <c r="F85" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -2579,10 +2579,10 @@
         <v>0.4249545</v>
       </c>
       <c r="E86" t="n">
+        <v>58.52589569160997</v>
+      </c>
+      <c r="F86" t="n">
         <v>0.3731749653816223</v>
-      </c>
-      <c r="F86" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -2604,10 +2604,10 @@
         <v>0.257906</v>
       </c>
       <c r="E87" t="n">
+        <v>58.97868480725624</v>
+      </c>
+      <c r="F87" t="n">
         <v>0.3199853897094727</v>
-      </c>
-      <c r="F87" t="n">
-        <v>1442.724609375</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -2629,10 +2629,10 @@
         <v>-0.440144</v>
       </c>
       <c r="E88" t="n">
+        <v>59.48952380952381</v>
+      </c>
+      <c r="F88" t="n">
         <v>0.2959308922290802</v>
-      </c>
-      <c r="F88" t="n">
-        <v>968.994140625</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -2654,10 +2654,10 @@
         <v>0.897729</v>
       </c>
       <c r="E89" t="n">
+        <v>1.160997732426304</v>
+      </c>
+      <c r="F89" t="n">
         <v>0.3756849765777588</v>
-      </c>
-      <c r="F89" t="n">
-        <v>430.6640625</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -2679,10 +2679,10 @@
         <v>1.393668</v>
       </c>
       <c r="E90" t="n">
+        <v>1.637006802721088</v>
+      </c>
+      <c r="F90" t="n">
         <v>0.324804961681366</v>
-      </c>
-      <c r="F90" t="n">
-        <v>409.130859375</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -2704,10 +2704,10 @@
         <v>-0.606958</v>
       </c>
       <c r="E91" t="n">
+        <v>4.446621315192743</v>
+      </c>
+      <c r="F91" t="n">
         <v>0.4582082331180573</v>
-      </c>
-      <c r="F91" t="n">
-        <v>387.59765625</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -2729,10 +2729,10 @@
         <v>0.102377</v>
       </c>
       <c r="E92" t="n">
+        <v>12.26013605442177</v>
+      </c>
+      <c r="F92" t="n">
         <v>0.5131728053092957</v>
-      </c>
-      <c r="F92" t="n">
-        <v>2002.587890625</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -2754,10 +2754,10 @@
         <v>-0.6829385000000001</v>
       </c>
       <c r="E93" t="n">
+        <v>13.67655328798186</v>
+      </c>
+      <c r="F93" t="n">
         <v>0.3681440055370331</v>
-      </c>
-      <c r="F93" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -2779,10 +2779,10 @@
         <v>-0.630756</v>
       </c>
       <c r="E94" t="n">
+        <v>16.70675736961451</v>
+      </c>
+      <c r="F94" t="n">
         <v>0.3775992691516876</v>
-      </c>
-      <c r="F94" t="n">
-        <v>624.462890625</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -2804,10 +2804,10 @@
         <v>0.1777462</v>
       </c>
       <c r="E95" t="n">
+        <v>17.0550566893424</v>
+      </c>
+      <c r="F95" t="n">
         <v>0.4056164920330048</v>
-      </c>
-      <c r="F95" t="n">
-        <v>2088.720703125</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -2829,10 +2829,10 @@
         <v>-0.07813899999999999</v>
       </c>
       <c r="E96" t="n">
+        <v>25.65804988662132</v>
+      </c>
+      <c r="F96" t="n">
         <v>0.3889858424663544</v>
-      </c>
-      <c r="F96" t="n">
-        <v>4069.775390625</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -2854,10 +2854,10 @@
         <v>-0.550197</v>
       </c>
       <c r="E97" t="n">
+        <v>26.86548752834467</v>
+      </c>
+      <c r="F97" t="n">
         <v>0.3980333805084229</v>
-      </c>
-      <c r="F97" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -2879,10 +2879,10 @@
         <v>-0.346654</v>
       </c>
       <c r="E98" t="n">
+        <v>27.44598639455782</v>
+      </c>
+      <c r="F98" t="n">
         <v>0.4524046778678894</v>
-      </c>
-      <c r="F98" t="n">
-        <v>4220.5078125</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -2904,10 +2904,10 @@
         <v>-0.444635</v>
       </c>
       <c r="E99" t="n">
+        <v>28.59537414965986</v>
+      </c>
+      <c r="F99" t="n">
         <v>0.3177550733089447</v>
-      </c>
-      <c r="F99" t="n">
-        <v>602.9296875</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>-0.81998876</v>
       </c>
       <c r="E100" t="n">
+        <v>30.499410430839</v>
+      </c>
+      <c r="F100" t="n">
         <v>0.3189653754234314</v>
-      </c>
-      <c r="F100" t="n">
-        <v>689.0625</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -2954,10 +2954,10 @@
         <v>0.824584</v>
       </c>
       <c r="E101" t="n">
+        <v>32.07836734693878</v>
+      </c>
+      <c r="F101" t="n">
         <v>0.2848235964775085</v>
-      </c>
-      <c r="F101" t="n">
-        <v>6890.625</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -2979,10 +2979,10 @@
         <v>-0.6653290000000001</v>
       </c>
       <c r="E102" t="n">
+        <v>32.67047619047619</v>
+      </c>
+      <c r="F102" t="n">
         <v>0.2379759103059769</v>
-      </c>
-      <c r="F102" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         <v>-0.453731</v>
       </c>
       <c r="E103" t="n">
+        <v>33.76181405895692</v>
+      </c>
+      <c r="F103" t="n">
         <v>0.2591888308525085</v>
-      </c>
-      <c r="F103" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -3029,10 +3029,10 @@
         <v>0.4260536</v>
       </c>
       <c r="E104" t="n">
+        <v>34.30748299319728</v>
+      </c>
+      <c r="F104" t="n">
         <v>0.289605975151062</v>
-      </c>
-      <c r="F104" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -3054,10 +3054,10 @@
         <v>0.009218800000000001</v>
       </c>
       <c r="E105" t="n">
+        <v>34.76027210884354</v>
+      </c>
+      <c r="F105" t="n">
         <v>0.3921566307544708</v>
-      </c>
-      <c r="F105" t="n">
-        <v>4198.974609375</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -3079,10 +3079,10 @@
         <v>-0.742829</v>
       </c>
       <c r="E106" t="n">
+        <v>35.77034013605442</v>
+      </c>
+      <c r="F106" t="n">
         <v>0.2818488776683807</v>
-      </c>
-      <c r="F106" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -3104,10 +3104,10 @@
         <v>-0.145613</v>
       </c>
       <c r="E107" t="n">
+        <v>36.22312925170068</v>
+      </c>
+      <c r="F107" t="n">
         <v>0.2680481672286987</v>
-      </c>
-      <c r="F107" t="n">
-        <v>1636.5234375</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -3129,10 +3129,10 @@
         <v>0.053713</v>
       </c>
       <c r="E108" t="n">
+        <v>37.3144671201814</v>
+      </c>
+      <c r="F108" t="n">
         <v>0.2711438238620758</v>
-      </c>
-      <c r="F108" t="n">
-        <v>861.328125</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -3154,10 +3154,10 @@
         <v>-0.445079</v>
       </c>
       <c r="E109" t="n">
+        <v>37.74403628117914</v>
+      </c>
+      <c r="F109" t="n">
         <v>0.2458178699016571</v>
-      </c>
-      <c r="F109" t="n">
-        <v>861.328125</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -3179,10 +3179,10 @@
         <v>-0.6327199999999999</v>
       </c>
       <c r="E110" t="n">
+        <v>38.22004535147392</v>
+      </c>
+      <c r="F110" t="n">
         <v>0.3928955793380737</v>
-      </c>
-      <c r="F110" t="n">
-        <v>8225.68359375</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -3204,10 +3204,10 @@
         <v>-0.7997529999999999</v>
       </c>
       <c r="E111" t="n">
+        <v>38.80054421768708</v>
+      </c>
+      <c r="F111" t="n">
         <v>0.3080992698669434</v>
-      </c>
-      <c r="F111" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -3229,10 +3229,10 @@
         <v>-0.13743768</v>
       </c>
       <c r="E112" t="n">
+        <v>39.23011337868481</v>
+      </c>
+      <c r="F112" t="n">
         <v>0.3900727033615112</v>
-      </c>
-      <c r="F112" t="n">
-        <v>4112.841796875</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -3254,10 +3254,10 @@
         <v>0.437813</v>
       </c>
       <c r="E113" t="n">
+        <v>39.82222222222222</v>
+      </c>
+      <c r="F113" t="n">
         <v>0.2952807247638702</v>
-      </c>
-      <c r="F113" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -3279,10 +3279,10 @@
         <v>0.936405</v>
       </c>
       <c r="E114" t="n">
+        <v>40.739410430839</v>
+      </c>
+      <c r="F114" t="n">
         <v>0.2276796698570251</v>
-      </c>
-      <c r="F114" t="n">
-        <v>882.861328125</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -3304,10 +3304,10 @@
         <v>0.9842850000000001</v>
       </c>
       <c r="E115" t="n">
+        <v>41.180589569161</v>
+      </c>
+      <c r="F115" t="n">
         <v>0.1846644133329391</v>
-      </c>
-      <c r="F115" t="n">
-        <v>1162.79296875</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -3329,10 +3329,10 @@
         <v>0.123661</v>
       </c>
       <c r="E116" t="n">
+        <v>41.63337868480725</v>
+      </c>
+      <c r="F116" t="n">
         <v>0.2363682687282562</v>
-      </c>
-      <c r="F116" t="n">
-        <v>6201.5625</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -3354,10 +3354,10 @@
         <v>-1.5515</v>
       </c>
       <c r="E117" t="n">
+        <v>42.55056689342403</v>
+      </c>
+      <c r="F117" t="n">
         <v>0.3407484292984009</v>
-      </c>
-      <c r="F117" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -3379,10 +3379,10 @@
         <v>-0.6481790000000001</v>
       </c>
       <c r="E118" t="n">
+        <v>43.46775510204082</v>
+      </c>
+      <c r="F118" t="n">
         <v>0.2753348648548126</v>
-      </c>
-      <c r="F118" t="n">
-        <v>818.26171875</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -3404,10 +3404,10 @@
         <v>0.2083894</v>
       </c>
       <c r="E119" t="n">
+        <v>44.09469387755102</v>
+      </c>
+      <c r="F119" t="n">
         <v>0.3038162887096405</v>
-      </c>
-      <c r="F119" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -3429,10 +3429,10 @@
         <v>0.120159</v>
       </c>
       <c r="E120" t="n">
+        <v>44.54748299319728</v>
+      </c>
+      <c r="F120" t="n">
         <v>0.2820907235145569</v>
-      </c>
-      <c r="F120" t="n">
-        <v>4177.44140625</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         <v>-0.0483341</v>
       </c>
       <c r="E121" t="n">
+        <v>45.47628117913832</v>
+      </c>
+      <c r="F121" t="n">
         <v>0.3166232705116272</v>
-      </c>
-      <c r="F121" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -3479,10 +3479,10 @@
         <v>0.432867</v>
       </c>
       <c r="E122" t="n">
+        <v>45.92907029478458</v>
+      </c>
+      <c r="F122" t="n">
         <v>0.2840993404388428</v>
-      </c>
-      <c r="F122" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -3504,10 +3504,10 @@
         <v>-0.01970600000000004</v>
       </c>
       <c r="E123" t="n">
+        <v>46.38185941043084</v>
+      </c>
+      <c r="F123" t="n">
         <v>0.2482411712408066</v>
-      </c>
-      <c r="F123" t="n">
-        <v>904.39453125</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -3529,10 +3529,10 @@
         <v>0.06030700000000001</v>
       </c>
       <c r="E124" t="n">
+        <v>46.85786848072562</v>
+      </c>
+      <c r="F124" t="n">
         <v>0.2277911454439163</v>
-      </c>
-      <c r="F124" t="n">
-        <v>4091.30859375</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -3554,10 +3554,10 @@
         <v>-0.6645</v>
       </c>
       <c r="E125" t="n">
+        <v>48.73868480725623</v>
+      </c>
+      <c r="F125" t="n">
         <v>0.1995283365249634</v>
-      </c>
-      <c r="F125" t="n">
-        <v>925.927734375</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -3579,10 +3579,10 @@
         <v>0.03965750000000001</v>
       </c>
       <c r="E126" t="n">
+        <v>49.66748299319728</v>
+      </c>
+      <c r="F126" t="n">
         <v>0.1713317632675171</v>
-      </c>
-      <c r="F126" t="n">
-        <v>4414.306640625</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -3604,10 +3604,10 @@
         <v>-0.119897</v>
       </c>
       <c r="E127" t="n">
+        <v>51.3277097505669</v>
+      </c>
+      <c r="F127" t="n">
         <v>0.183479055762291</v>
-      </c>
-      <c r="F127" t="n">
-        <v>904.39453125</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -3629,10 +3629,10 @@
         <v>-0.0705794</v>
       </c>
       <c r="E128" t="n">
+        <v>51.66439909297052</v>
+      </c>
+      <c r="F128" t="n">
         <v>0.2579222321510315</v>
-      </c>
-      <c r="F128" t="n">
-        <v>4414.306640625</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -3654,10 +3654,10 @@
         <v>-0.404515</v>
       </c>
       <c r="E129" t="n">
+        <v>53.52199546485261</v>
+      </c>
+      <c r="F129" t="n">
         <v>0.2905837893486023</v>
-      </c>
-      <c r="F129" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -3679,10 +3679,10 @@
         <v>0.048535</v>
       </c>
       <c r="E130" t="n">
+        <v>53.97478458049886</v>
+      </c>
+      <c r="F130" t="n">
         <v>0.3086844682693481</v>
-      </c>
-      <c r="F130" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -3704,10 +3704,10 @@
         <v>0.369152</v>
       </c>
       <c r="E131" t="n">
+        <v>54.54367346938776</v>
+      </c>
+      <c r="F131" t="n">
         <v>0.3014267385005951</v>
-      </c>
-      <c r="F131" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -3729,10 +3729,10 @@
         <v>-0.26055892</v>
       </c>
       <c r="E132" t="n">
+        <v>55.58857142857143</v>
+      </c>
+      <c r="F132" t="n">
         <v>0.262865424156189</v>
-      </c>
-      <c r="F132" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -3754,10 +3754,10 @@
         <v>-0.0585232</v>
       </c>
       <c r="E133" t="n">
+        <v>55.9136507936508</v>
+      </c>
+      <c r="F133" t="n">
         <v>0.2608446776866913</v>
-      </c>
-      <c r="F133" t="n">
-        <v>4220.5078125</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -3779,10 +3779,10 @@
         <v>-0.31922255</v>
       </c>
       <c r="E134" t="n">
+        <v>56.6334693877551</v>
+      </c>
+      <c r="F134" t="n">
         <v>0.2469711750745773</v>
-      </c>
-      <c r="F134" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -3804,10 +3804,10 @@
         <v>0.4965579999999999</v>
       </c>
       <c r="E135" t="n">
+        <v>57.15591836734694</v>
+      </c>
+      <c r="F135" t="n">
         <v>0.258684366941452</v>
-      </c>
-      <c r="F135" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -3829,10 +3829,10 @@
         <v>0.541127</v>
       </c>
       <c r="E136" t="n">
+        <v>57.63192743764172</v>
+      </c>
+      <c r="F136" t="n">
         <v>0.2520054876804352</v>
-      </c>
-      <c r="F136" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -3854,10 +3854,10 @@
         <v>-0.70282975</v>
       </c>
       <c r="E137" t="n">
+        <v>58.10793650793651</v>
+      </c>
+      <c r="F137" t="n">
         <v>0.2659854590892792</v>
-      </c>
-      <c r="F137" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -3879,10 +3879,10 @@
         <v>0.007268000000000012</v>
       </c>
       <c r="E138" t="n">
+        <v>58.63038548752834</v>
+      </c>
+      <c r="F138" t="n">
         <v>0.2628146708011627</v>
-      </c>
-      <c r="F138" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -3904,10 +3904,10 @@
         <v>-0.547608</v>
       </c>
       <c r="E139" t="n">
+        <v>59.58240362811792</v>
+      </c>
+      <c r="F139" t="n">
         <v>0.2154809534549713</v>
-      </c>
-      <c r="F139" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -3929,10 +3929,10 @@
         <v>-0.4547450000000001</v>
       </c>
       <c r="E140" t="n">
+        <v>3.13469387755102</v>
+      </c>
+      <c r="F140" t="n">
         <v>0.4501658380031586</v>
-      </c>
-      <c r="F140" t="n">
-        <v>3746.77734375</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         <v>0.2678372</v>
       </c>
       <c r="E141" t="n">
+        <v>3.773242630385488</v>
+      </c>
+      <c r="F141" t="n">
         <v>0.6074351072311401</v>
-      </c>
-      <c r="F141" t="n">
-        <v>430.6640625</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -3979,10 +3979,10 @@
         <v>-0.99444</v>
       </c>
       <c r="E142" t="n">
+        <v>4.400181405895691</v>
+      </c>
+      <c r="F142" t="n">
         <v>0.6542943716049194</v>
-      </c>
-      <c r="F142" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -4004,10 +4004,10 @@
         <v>-0.2159526</v>
       </c>
       <c r="E143" t="n">
+        <v>5.061950113378685</v>
+      </c>
+      <c r="F143" t="n">
         <v>0.563585102558136</v>
-      </c>
-      <c r="F143" t="n">
-        <v>2282.51953125</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -4029,10 +4029,10 @@
         <v>0.416245</v>
       </c>
       <c r="E144" t="n">
+        <v>5.712108843537415</v>
+      </c>
+      <c r="F144" t="n">
         <v>0.5068813562393188</v>
-      </c>
-      <c r="F144" t="n">
-        <v>301.46484375</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -4054,10 +4054,10 @@
         <v>-0.036271</v>
       </c>
       <c r="E145" t="n">
+        <v>6.443537414965986</v>
+      </c>
+      <c r="F145" t="n">
         <v>0.6627400517463684</v>
-      </c>
-      <c r="F145" t="n">
-        <v>322.998046875</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -4079,10 +4079,10 @@
         <v>0.325368</v>
       </c>
       <c r="E146" t="n">
+        <v>6.989206349206349</v>
+      </c>
+      <c r="F146" t="n">
         <v>0.5718967318534851</v>
-      </c>
-      <c r="F146" t="n">
-        <v>3552.978515625</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
@@ -4104,10 +4104,10 @@
         <v>2.046695</v>
       </c>
       <c r="E147" t="n">
+        <v>8.916462585034013</v>
+      </c>
+      <c r="F147" t="n">
         <v>0.6470839381217957</v>
-      </c>
-      <c r="F147" t="n">
-        <v>279.931640625</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -4129,10 +4129,10 @@
         <v>-0.3310078</v>
       </c>
       <c r="E148" t="n">
+        <v>9.287981859410431</v>
+      </c>
+      <c r="F148" t="n">
         <v>0.5898582339286804</v>
-      </c>
-      <c r="F148" t="n">
-        <v>2971.58203125</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -4154,10 +4154,10 @@
         <v>-0.298349</v>
       </c>
       <c r="E149" t="n">
+        <v>10.27482993197279</v>
+      </c>
+      <c r="F149" t="n">
         <v>0.6630143523216248</v>
-      </c>
-      <c r="F149" t="n">
-        <v>3445.3125</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -4179,10 +4179,10 @@
         <v>-0.1466784</v>
       </c>
       <c r="E150" t="n">
+        <v>11.98149659863946</v>
+      </c>
+      <c r="F150" t="n">
         <v>0.4297657012939453</v>
-      </c>
-      <c r="F150" t="n">
-        <v>3466.845703125</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -4204,10 +4204,10 @@
         <v>-0.205091</v>
       </c>
       <c r="E151" t="n">
+        <v>12.80580498866213</v>
+      </c>
+      <c r="F151" t="n">
         <v>0.6639760732650757</v>
-      </c>
-      <c r="F151" t="n">
-        <v>301.46484375</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -4229,10 +4229,10 @@
         <v>-1.023535</v>
       </c>
       <c r="E152" t="n">
+        <v>13.47918367346939</v>
+      </c>
+      <c r="F152" t="n">
         <v>0.6396822333335876</v>
-      </c>
-      <c r="F152" t="n">
-        <v>344.53125</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -4254,10 +4254,10 @@
         <v>-0.12648865</v>
       </c>
       <c r="E153" t="n">
+        <v>14.0712925170068</v>
+      </c>
+      <c r="F153" t="n">
         <v>0.5078771710395813</v>
-      </c>
-      <c r="F153" t="n">
-        <v>3682.177734375</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -4279,10 +4279,10 @@
         <v>-1.663716</v>
       </c>
       <c r="E154" t="n">
+        <v>16.02176870748299</v>
+      </c>
+      <c r="F154" t="n">
         <v>0.613507866859436</v>
-      </c>
-      <c r="F154" t="n">
-        <v>301.46484375</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -4304,10 +4304,10 @@
         <v>-0.378903</v>
       </c>
       <c r="E155" t="n">
+        <v>16.68353741496599</v>
+      </c>
+      <c r="F155" t="n">
         <v>0.6802361011505127</v>
-      </c>
-      <c r="F155" t="n">
-        <v>387.59765625</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -4329,10 +4329,10 @@
         <v>0.120544</v>
       </c>
       <c r="E156" t="n">
+        <v>17.10149659863946</v>
+      </c>
+      <c r="F156" t="n">
         <v>0.5199732184410095</v>
-      </c>
-      <c r="F156" t="n">
-        <v>3402.24609375</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -4354,10 +4354,10 @@
         <v>-0.1135084</v>
       </c>
       <c r="E157" t="n">
+        <v>17.96063492063492</v>
+      </c>
+      <c r="F157" t="n">
         <v>0.5439461469650269</v>
-      </c>
-      <c r="F157" t="n">
-        <v>3380.712890625</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -4379,10 +4379,10 @@
         <v>0.0590746</v>
       </c>
       <c r="E158" t="n">
+        <v>19.4118820861678</v>
+      </c>
+      <c r="F158" t="n">
         <v>0.4842812716960907</v>
-      </c>
-      <c r="F158" t="n">
-        <v>2519.384765625</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -4404,10 +4404,10 @@
         <v>-1.0059392</v>
       </c>
       <c r="E159" t="n">
+        <v>20.02721088435374</v>
+      </c>
+      <c r="F159" t="n">
         <v>0.6011495590209961</v>
-      </c>
-      <c r="F159" t="n">
-        <v>301.46484375</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -4429,10 +4429,10 @@
         <v>-0.5397606</v>
       </c>
       <c r="E160" t="n">
+        <v>20.56126984126984</v>
+      </c>
+      <c r="F160" t="n">
         <v>0.6858065724372864</v>
-      </c>
-      <c r="F160" t="n">
-        <v>279.931640625</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -4454,10 +4454,10 @@
         <v>-0.2532152</v>
       </c>
       <c r="E161" t="n">
+        <v>22.86004535147392</v>
+      </c>
+      <c r="F161" t="n">
         <v>0.5833697319030762</v>
-      </c>
-      <c r="F161" t="n">
-        <v>3337.646484375</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -4479,10 +4479,10 @@
         <v>0.153175</v>
       </c>
       <c r="E162" t="n">
+        <v>25.40263038548753</v>
+      </c>
+      <c r="F162" t="n">
         <v>0.5411797165870667</v>
-      </c>
-      <c r="F162" t="n">
-        <v>3186.9140625</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -4504,10 +4504,10 @@
         <v>0.2147085</v>
       </c>
       <c r="E163" t="n">
+        <v>28.09614512471655</v>
+      </c>
+      <c r="F163" t="n">
         <v>0.3982822895050049</v>
-      </c>
-      <c r="F163" t="n">
-        <v>2239.453125</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -4529,10 +4529,10 @@
         <v>-0.214564</v>
       </c>
       <c r="E164" t="n">
+        <v>29.83764172335601</v>
+      </c>
+      <c r="F164" t="n">
         <v>0.4441517889499664</v>
-      </c>
-      <c r="F164" t="n">
-        <v>3574.51171875</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -4554,10 +4554,10 @@
         <v>0.342455</v>
       </c>
       <c r="E165" t="n">
+        <v>32.34539682539683</v>
+      </c>
+      <c r="F165" t="n">
         <v>0.5341187119483948</v>
-      </c>
-      <c r="F165" t="n">
-        <v>3660.64453125</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -4579,10 +4579,10 @@
         <v>-0.1456514</v>
       </c>
       <c r="E166" t="n">
+        <v>35.49170068027211</v>
+      </c>
+      <c r="F166" t="n">
         <v>0.6634252667427063</v>
-      </c>
-      <c r="F166" t="n">
-        <v>2282.51953125</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -4604,10 +4604,10 @@
         <v>-0.06178</v>
       </c>
       <c r="E167" t="n">
+        <v>37.58149659863945</v>
+      </c>
+      <c r="F167" t="n">
         <v>0.4867027997970581</v>
-      </c>
-      <c r="F167" t="n">
-        <v>2454.78515625</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -4629,10 +4629,10 @@
         <v>-0.1531305</v>
       </c>
       <c r="E168" t="n">
+        <v>42.29514739229025</v>
+      </c>
+      <c r="F168" t="n">
         <v>0.5347205400466919</v>
-      </c>
-      <c r="F168" t="n">
-        <v>3337.646484375</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         <v>-0.114003</v>
       </c>
       <c r="E169" t="n">
+        <v>45.39501133786848</v>
+      </c>
+      <c r="F169" t="n">
         <v>0.5817247629165649</v>
-      </c>
-      <c r="F169" t="n">
-        <v>3466.845703125</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -4679,10 +4679,10 @@
         <v>0.0907955</v>
       </c>
       <c r="E170" t="n">
+        <v>47.03201814058957</v>
+      </c>
+      <c r="F170" t="n">
         <v>0.5353156924247742</v>
-      </c>
-      <c r="F170" t="n">
-        <v>2260.986328125</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -4704,10 +4704,10 @@
         <v>-0.150888</v>
       </c>
       <c r="E171" t="n">
+        <v>48.56453514739229</v>
+      </c>
+      <c r="F171" t="n">
         <v>0.5287635922431946</v>
-      </c>
-      <c r="F171" t="n">
-        <v>3423.779296875</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -4729,10 +4729,10 @@
         <v>0.4448744</v>
       </c>
       <c r="E172" t="n">
+        <v>51.83854875283447</v>
+      </c>
+      <c r="F172" t="n">
         <v>0.5457456111907959</v>
-      </c>
-      <c r="F172" t="n">
-        <v>2519.384765625</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -4754,10 +4754,10 @@
         <v>0.492539</v>
       </c>
       <c r="E173" t="n">
+        <v>52.51192743764172</v>
+      </c>
+      <c r="F173" t="n">
         <v>0.5469157099723816</v>
-      </c>
-      <c r="F173" t="n">
-        <v>452.197265625</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -4779,10 +4779,10 @@
         <v>-0.0162183</v>
       </c>
       <c r="E174" t="n">
+        <v>52.99954648526077</v>
+      </c>
+      <c r="F174" t="n">
         <v>0.5064195394515991</v>
-      </c>
-      <c r="F174" t="n">
-        <v>409.130859375</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -4804,10 +4804,10 @@
         <v>0.3592150000000001</v>
       </c>
       <c r="E175" t="n">
+        <v>53.67292517006803</v>
+      </c>
+      <c r="F175" t="n">
         <v>0.4942649900913239</v>
-      </c>
-      <c r="F175" t="n">
-        <v>387.59765625</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -4829,10 +4829,10 @@
         <v>-0.0570052</v>
       </c>
       <c r="E176" t="n">
+        <v>54.77587301587302</v>
+      </c>
+      <c r="F176" t="n">
         <v>0.5133434534072876</v>
-      </c>
-      <c r="F176" t="n">
-        <v>2260.986328125</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -4854,10 +4854,10 @@
         <v>-0.0667985</v>
       </c>
       <c r="E177" t="n">
+        <v>55.7859410430839</v>
+      </c>
+      <c r="F177" t="n">
         <v>0.4293949604034424</v>
-      </c>
-      <c r="F177" t="n">
-        <v>452.197265625</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -4879,10 +4879,10 @@
         <v>-0.2745124</v>
       </c>
       <c r="E178" t="n">
+        <v>56.26195011337869</v>
+      </c>
+      <c r="F178" t="n">
         <v>0.4842788279056549</v>
-      </c>
-      <c r="F178" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         <v>0.03380160000000001</v>
       </c>
       <c r="E179" t="n">
+        <v>56.62185941043084</v>
+      </c>
+      <c r="F179" t="n">
         <v>0.5600021481513977</v>
-      </c>
-      <c r="F179" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -4929,10 +4929,10 @@
         <v>-0.2425672</v>
       </c>
       <c r="E180" t="n">
+        <v>57.20235827664399</v>
+      </c>
+      <c r="F180" t="n">
         <v>0.4596482515335083</v>
-      </c>
-      <c r="F180" t="n">
-        <v>2282.51953125</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -4954,10 +4954,10 @@
         <v>1.01148</v>
       </c>
       <c r="E181" t="n">
+        <v>57.65514739229025</v>
+      </c>
+      <c r="F181" t="n">
         <v>0.4429691433906555</v>
-      </c>
-      <c r="F181" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -4979,10 +4979,10 @@
         <v>0.417074</v>
       </c>
       <c r="E182" t="n">
+        <v>58.09632653061225</v>
+      </c>
+      <c r="F182" t="n">
         <v>0.4564569890499115</v>
-      </c>
-      <c r="F182" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -5004,10 +5004,10 @@
         <v>-0.080842</v>
       </c>
       <c r="E183" t="n">
+        <v>58.53750566893424</v>
+      </c>
+      <c r="F183" t="n">
         <v>0.5287003517150879</v>
-      </c>
-      <c r="F183" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -5029,10 +5029,10 @@
         <v>0.1253174</v>
       </c>
       <c r="E184" t="n">
+        <v>58.96707482993197</v>
+      </c>
+      <c r="F184" t="n">
         <v>0.5381126999855042</v>
-      </c>
-      <c r="F184" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -5054,10 +5054,10 @@
         <v>0.03648169999999996</v>
       </c>
       <c r="E185" t="n">
+        <v>59.68689342403628</v>
+      </c>
+      <c r="F185" t="n">
         <v>0.4912011623382568</v>
-      </c>
-      <c r="F185" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -5079,10 +5079,10 @@
         <v>-0.15634</v>
       </c>
       <c r="E186" t="n">
+        <v>1.555736961451247</v>
+      </c>
+      <c r="F186" t="n">
         <v>0.4746626615524292</v>
-      </c>
-      <c r="F186" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -5104,10 +5104,10 @@
         <v>0.297729</v>
       </c>
       <c r="E187" t="n">
+        <v>4.121541950113379</v>
+      </c>
+      <c r="F187" t="n">
         <v>0.4383725225925446</v>
-      </c>
-      <c r="F187" t="n">
-        <v>4155.908203125</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -5129,10 +5129,10 @@
         <v>-0.657796</v>
       </c>
       <c r="E188" t="n">
+        <v>6.965986394557823</v>
+      </c>
+      <c r="F188" t="n">
         <v>0.450365424156189</v>
-      </c>
-      <c r="F188" t="n">
-        <v>732.12890625</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -5154,10 +5154,10 @@
         <v>0.05792969999999999</v>
       </c>
       <c r="E189" t="n">
+        <v>7.430385487528345</v>
+      </c>
+      <c r="F189" t="n">
         <v>0.4416683912277222</v>
-      </c>
-      <c r="F189" t="n">
-        <v>775.1953125</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -5179,10 +5179,10 @@
         <v>0.02921700000000002</v>
       </c>
       <c r="E190" t="n">
+        <v>7.976054421768707</v>
+      </c>
+      <c r="F190" t="n">
         <v>0.4668835401535034</v>
-      </c>
-      <c r="F190" t="n">
-        <v>710.595703125</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -5204,10 +5204,10 @@
         <v>0.212675</v>
       </c>
       <c r="E191" t="n">
+        <v>8.324353741496598</v>
+      </c>
+      <c r="F191" t="n">
         <v>0.4125043451786041</v>
-      </c>
-      <c r="F191" t="n">
-        <v>4608.10546875</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -5229,10 +5229,10 @@
         <v>0.1060552</v>
       </c>
       <c r="E192" t="n">
+        <v>12.97995464852608</v>
+      </c>
+      <c r="F192" t="n">
         <v>0.344047337770462</v>
-      </c>
-      <c r="F192" t="n">
-        <v>4112.841796875</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -5254,10 +5254,10 @@
         <v>0.013914</v>
       </c>
       <c r="E193" t="n">
+        <v>15.56897959183673</v>
+      </c>
+      <c r="F193" t="n">
         <v>0.3357683718204498</v>
-      </c>
-      <c r="F193" t="n">
-        <v>3186.9140625</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -5279,10 +5279,10 @@
         <v>-0.848939</v>
       </c>
       <c r="E194" t="n">
+        <v>19.73696145124716</v>
+      </c>
+      <c r="F194" t="n">
         <v>0.4396944940090179</v>
-      </c>
-      <c r="F194" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -5304,10 +5304,10 @@
         <v>0.188291</v>
       </c>
       <c r="E195" t="n">
+        <v>20.1665306122449</v>
+      </c>
+      <c r="F195" t="n">
         <v>0.4782217442989349</v>
-      </c>
-      <c r="F195" t="n">
-        <v>4780.37109375</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -5329,10 +5329,10 @@
         <v>0.0605255</v>
       </c>
       <c r="E196" t="n">
+        <v>22.8368253968254</v>
+      </c>
+      <c r="F196" t="n">
         <v>0.4556012749671936</v>
-      </c>
-      <c r="F196" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -5354,10 +5354,10 @@
         <v>-0.161999</v>
       </c>
       <c r="E197" t="n">
+        <v>23.28961451247165</v>
+      </c>
+      <c r="F197" t="n">
         <v>0.3935619294643402</v>
-      </c>
-      <c r="F197" t="n">
-        <v>1421.19140625</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -5379,10 +5379,10 @@
         <v>0.346434</v>
       </c>
       <c r="E198" t="n">
+        <v>24.26485260770975</v>
+      </c>
+      <c r="F198" t="n">
         <v>0.454278290271759</v>
-      </c>
-      <c r="F198" t="n">
-        <v>3165.380859375</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -5404,10 +5404,10 @@
         <v>0.146737</v>
       </c>
       <c r="E199" t="n">
+        <v>24.86857142857143</v>
+      </c>
+      <c r="F199" t="n">
         <v>0.4445548057556152</v>
-      </c>
-      <c r="F199" t="n">
-        <v>4091.30859375</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -5429,10 +5429,10 @@
         <v>-0.212387</v>
       </c>
       <c r="E200" t="n">
+        <v>27.89877551020408</v>
+      </c>
+      <c r="F200" t="n">
         <v>0.4055695533752441</v>
-      </c>
-      <c r="F200" t="n">
-        <v>4435.83984375</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -5454,10 +5454,10 @@
         <v>-0.08472499999999998</v>
       </c>
       <c r="E201" t="n">
+        <v>29.41968253968254</v>
+      </c>
+      <c r="F201" t="n">
         <v>0.3914630115032196</v>
-      </c>
-      <c r="F201" t="n">
-        <v>4220.5078125</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -5479,10 +5479,10 @@
         <v>0.214525</v>
       </c>
       <c r="E202" t="n">
+        <v>32.33378684807256</v>
+      </c>
+      <c r="F202" t="n">
         <v>0.5157358646392822</v>
-      </c>
-      <c r="F202" t="n">
-        <v>3251.513671875</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -5504,10 +5504,10 @@
         <v>-0.00136300000000001</v>
       </c>
       <c r="E203" t="n">
+        <v>33.73859410430839</v>
+      </c>
+      <c r="F203" t="n">
         <v>0.4191933870315552</v>
-      </c>
-      <c r="F203" t="n">
-        <v>4198.974609375</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -5529,10 +5529,10 @@
         <v>-0.159544</v>
       </c>
       <c r="E204" t="n">
+        <v>35.64263038548753</v>
+      </c>
+      <c r="F204" t="n">
         <v>0.492092490196228</v>
-      </c>
-      <c r="F204" t="n">
-        <v>3014.6484375</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -5554,10 +5554,10 @@
         <v>0.182578</v>
       </c>
       <c r="E205" t="n">
+        <v>38.87020408163265</v>
+      </c>
+      <c r="F205" t="n">
         <v>0.3671734929084778</v>
-      </c>
-      <c r="F205" t="n">
-        <v>4995.703125</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -5579,10 +5579,10 @@
         <v>-0.43567</v>
       </c>
       <c r="E206" t="n">
+        <v>39.47392290249433</v>
+      </c>
+      <c r="F206" t="n">
         <v>0.412855476140976</v>
-      </c>
-      <c r="F206" t="n">
-        <v>2993.115234375</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -5604,10 +5604,10 @@
         <v>0.0151313</v>
       </c>
       <c r="E207" t="n">
+        <v>42.72471655328798</v>
+      </c>
+      <c r="F207" t="n">
         <v>0.4161770343780518</v>
-      </c>
-      <c r="F207" t="n">
-        <v>3100.78125</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -5629,10 +5629,10 @@
         <v>0.156424</v>
       </c>
       <c r="E208" t="n">
+        <v>44.50104308390023</v>
+      </c>
+      <c r="F208" t="n">
         <v>0.3906069099903107</v>
-      </c>
-      <c r="F208" t="n">
-        <v>3466.845703125</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -5654,10 +5654,10 @@
         <v>-0.08558900000000001</v>
       </c>
       <c r="E209" t="n">
+        <v>47.9956462585034</v>
+      </c>
+      <c r="F209" t="n">
         <v>0.5165995359420776</v>
-      </c>
-      <c r="F209" t="n">
-        <v>3466.845703125</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -5679,10 +5679,10 @@
         <v>0.02102030000000001</v>
       </c>
       <c r="E210" t="n">
+        <v>48.98249433106576</v>
+      </c>
+      <c r="F210" t="n">
         <v>0.4706869423389435</v>
-      </c>
-      <c r="F210" t="n">
-        <v>3423.779296875</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -5704,10 +5704,10 @@
         <v>0.241376</v>
       </c>
       <c r="E211" t="n">
+        <v>49.89968253968254</v>
+      </c>
+      <c r="F211" t="n">
         <v>0.428582489490509</v>
-      </c>
-      <c r="F211" t="n">
-        <v>2928.515625</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -5729,10 +5729,10 @@
         <v>0.06816069999999996</v>
       </c>
       <c r="E212" t="n">
+        <v>52.41904761904762</v>
+      </c>
+      <c r="F212" t="n">
         <v>0.4263865649700165</v>
-      </c>
-      <c r="F212" t="n">
-        <v>9280.810546875</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
@@ -5754,10 +5754,10 @@
         <v>-0.1487746</v>
       </c>
       <c r="E213" t="n">
+        <v>55.85560090702948</v>
+      </c>
+      <c r="F213" t="n">
         <v>0.5258585214614868</v>
-      </c>
-      <c r="F213" t="n">
-        <v>2842.3828125</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
@@ -5779,10 +5779,10 @@
         <v>0.08279</v>
       </c>
       <c r="E214" t="n">
+        <v>59.44308390022676</v>
+      </c>
+      <c r="F214" t="n">
         <v>0.3879822492599487</v>
-      </c>
-      <c r="F214" t="n">
-        <v>3875.9765625</v>
       </c>
       <c r="G214" t="inlineStr">
         <is>
@@ -5804,10 +5804,10 @@
         <v>0.6026659999999999</v>
       </c>
       <c r="E215" t="n">
+        <v>0.08126984126984127</v>
+      </c>
+      <c r="F215" t="n">
         <v>0.4353636801242828</v>
-      </c>
-      <c r="F215" t="n">
-        <v>366.064453125</v>
       </c>
       <c r="G215" t="inlineStr">
         <is>
@@ -5829,10 +5829,10 @@
         <v>-0.3020942</v>
       </c>
       <c r="E216" t="n">
+        <v>0.5340589569160997</v>
+      </c>
+      <c r="F216" t="n">
         <v>0.3794967532157898</v>
-      </c>
-      <c r="F216" t="n">
-        <v>3488.37890625</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         <v>-0.3084</v>
       </c>
       <c r="E217" t="n">
+        <v>1.126167800453515</v>
+      </c>
+      <c r="F217" t="n">
         <v>0.4570063948631287</v>
-      </c>
-      <c r="F217" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G217" t="inlineStr">
         <is>
@@ -5879,10 +5879,10 @@
         <v>0.117156</v>
       </c>
       <c r="E218" t="n">
+        <v>2.832834467120181</v>
+      </c>
+      <c r="F218" t="n">
         <v>0.4389214515686035</v>
-      </c>
-      <c r="F218" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G218" t="inlineStr">
         <is>
@@ -5904,10 +5904,10 @@
         <v>-0.9678909999999998</v>
       </c>
       <c r="E219" t="n">
+        <v>3.297233560090703</v>
+      </c>
+      <c r="F219" t="n">
         <v>0.486061155796051</v>
-      </c>
-      <c r="F219" t="n">
-        <v>645.99609375</v>
       </c>
       <c r="G219" t="inlineStr">
         <is>
@@ -5929,10 +5929,10 @@
         <v>-0.0923494</v>
       </c>
       <c r="E220" t="n">
+        <v>4.818140589569161</v>
+      </c>
+      <c r="F220" t="n">
         <v>0.4669179320335388</v>
-      </c>
-      <c r="F220" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G220" t="inlineStr">
         <is>
@@ -5954,10 +5954,10 @@
         <v>-0.0252111</v>
       </c>
       <c r="E221" t="n">
+        <v>5.270929705215419</v>
+      </c>
+      <c r="F221" t="n">
         <v>0.3738939762115479</v>
-      </c>
-      <c r="F221" t="n">
-        <v>753.662109375</v>
       </c>
       <c r="G221" t="inlineStr">
         <is>
@@ -5979,10 +5979,10 @@
         <v>-0.274236</v>
       </c>
       <c r="E222" t="n">
+        <v>5.758548752834467</v>
+      </c>
+      <c r="F222" t="n">
         <v>0.4111570715904236</v>
-      </c>
-      <c r="F222" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G222" t="inlineStr">
         <is>
@@ -6004,10 +6004,10 @@
         <v>0.0191025</v>
       </c>
       <c r="E223" t="n">
+        <v>7.267845804988662</v>
+      </c>
+      <c r="F223" t="n">
         <v>0.4562970995903015</v>
-      </c>
-      <c r="F223" t="n">
-        <v>624.462890625</v>
       </c>
       <c r="G223" t="inlineStr">
         <is>
@@ -6029,10 +6029,10 @@
         <v>-0.780322</v>
       </c>
       <c r="E224" t="n">
+        <v>7.767074829931973</v>
+      </c>
+      <c r="F224" t="n">
         <v>0.4465092420578003</v>
-      </c>
-      <c r="F224" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G224" t="inlineStr">
         <is>
@@ -6054,10 +6054,10 @@
         <v>0.5041330000000001</v>
       </c>
       <c r="E225" t="n">
+        <v>8.324353741496598</v>
+      </c>
+      <c r="F225" t="n">
         <v>0.4197844564914703</v>
-      </c>
-      <c r="F225" t="n">
-        <v>2993.115234375</v>
       </c>
       <c r="G225" t="inlineStr">
         <is>
@@ -6079,10 +6079,10 @@
         <v>0.3316250000000001</v>
       </c>
       <c r="E226" t="n">
+        <v>9.833650793650794</v>
+      </c>
+      <c r="F226" t="n">
         <v>0.4612756073474884</v>
-      </c>
-      <c r="F226" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G226" t="inlineStr">
         <is>
@@ -6104,10 +6104,10 @@
         <v>0.1597845</v>
       </c>
       <c r="E227" t="n">
+        <v>10.32126984126984</v>
+      </c>
+      <c r="F227" t="n">
         <v>0.494004100561142</v>
-      </c>
-      <c r="F227" t="n">
-        <v>1442.724609375</v>
       </c>
       <c r="G227" t="inlineStr">
         <is>
@@ -6129,10 +6129,10 @@
         <v>-0.8898569999999999</v>
       </c>
       <c r="E228" t="n">
+        <v>11.36616780045351</v>
+      </c>
+      <c r="F228" t="n">
         <v>0.4643582701683044</v>
-      </c>
-      <c r="F228" t="n">
-        <v>409.130859375</v>
       </c>
       <c r="G228" t="inlineStr">
         <is>
@@ -6154,10 +6154,10 @@
         <v>-0.0290865</v>
       </c>
       <c r="E229" t="n">
+        <v>11.90022675736961</v>
+      </c>
+      <c r="F229" t="n">
         <v>0.4131926298141479</v>
-      </c>
-      <c r="F229" t="n">
-        <v>2928.515625</v>
       </c>
       <c r="G229" t="inlineStr">
         <is>
@@ -6179,10 +6179,10 @@
         <v>0.8504930000000001</v>
       </c>
       <c r="E230" t="n">
+        <v>12.45750566893424</v>
+      </c>
+      <c r="F230" t="n">
         <v>0.46224644780159</v>
-      </c>
-      <c r="F230" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G230" t="inlineStr">
         <is>
@@ -6204,10 +6204,10 @@
         <v>-0.806961</v>
       </c>
       <c r="E231" t="n">
+        <v>13.46757369614513</v>
+      </c>
+      <c r="F231" t="n">
         <v>0.4818947315216064</v>
-      </c>
-      <c r="F231" t="n">
-        <v>430.6640625</v>
       </c>
       <c r="G231" t="inlineStr">
         <is>
@@ -6229,10 +6229,10 @@
         <v>0.008760000000000006</v>
       </c>
       <c r="E232" t="n">
+        <v>14.02485260770975</v>
+      </c>
+      <c r="F232" t="n">
         <v>0.4708978533744812</v>
-      </c>
-      <c r="F232" t="n">
-        <v>2756.25</v>
       </c>
       <c r="G232" t="inlineStr">
         <is>
@@ -6254,10 +6254,10 @@
         <v>0.280993</v>
       </c>
       <c r="E233" t="n">
+        <v>15.71990929705215</v>
+      </c>
+      <c r="F233" t="n">
         <v>0.2222174108028412</v>
-      </c>
-      <c r="F233" t="n">
-        <v>2820.849609375</v>
       </c>
       <c r="G233" t="inlineStr">
         <is>
@@ -6279,10 +6279,10 @@
         <v>-0.561734</v>
       </c>
       <c r="E234" t="n">
+        <v>18.85460317460317</v>
+      </c>
+      <c r="F234" t="n">
         <v>0.3909539580345154</v>
-      </c>
-      <c r="F234" t="n">
-        <v>1701.123046875</v>
       </c>
       <c r="G234" t="inlineStr">
         <is>
@@ -6304,10 +6304,10 @@
         <v>-0.8348059999999999</v>
       </c>
       <c r="E235" t="n">
+        <v>19.87628117913832</v>
+      </c>
+      <c r="F235" t="n">
         <v>0.5702017545700073</v>
-      </c>
-      <c r="F235" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G235" t="inlineStr">
         <is>
@@ -6329,10 +6329,10 @@
         <v>-0.128901</v>
       </c>
       <c r="E236" t="n">
+        <v>20.00399092970521</v>
+      </c>
+      <c r="F236" t="n">
         <v>0.5974416732788086</v>
-      </c>
-      <c r="F236" t="n">
-        <v>2088.720703125</v>
       </c>
       <c r="G236" t="inlineStr">
         <is>
@@ -6354,10 +6354,10 @@
         <v>0.62644</v>
       </c>
       <c r="E237" t="n">
+        <v>21.43201814058957</v>
+      </c>
+      <c r="F237" t="n">
         <v>0.5014625787734985</v>
-      </c>
-      <c r="F237" t="n">
-        <v>430.6640625</v>
       </c>
       <c r="G237" t="inlineStr">
         <is>
@@ -6379,10 +6379,10 @@
         <v>0.236481</v>
       </c>
       <c r="E238" t="n">
+        <v>21.93124716553288</v>
+      </c>
+      <c r="F238" t="n">
         <v>0.4648246765136719</v>
-      </c>
-      <c r="F238" t="n">
-        <v>387.59765625</v>
       </c>
       <c r="G238" t="inlineStr">
         <is>
@@ -6404,10 +6404,10 @@
         <v>-0.32201</v>
       </c>
       <c r="E239" t="n">
+        <v>22.59301587301587</v>
+      </c>
+      <c r="F239" t="n">
         <v>0.4084689319133759</v>
-      </c>
-      <c r="F239" t="n">
-        <v>3337.646484375</v>
       </c>
       <c r="G239" t="inlineStr">
         <is>
@@ -6429,10 +6429,10 @@
         <v>-0.025684</v>
       </c>
       <c r="E240" t="n">
+        <v>25.95990929705215</v>
+      </c>
+      <c r="F240" t="n">
         <v>0.3658051192760468</v>
-      </c>
-      <c r="F240" t="n">
-        <v>2411.71875</v>
       </c>
       <c r="G240" t="inlineStr">
         <is>
@@ -6454,10 +6454,10 @@
         <v>-0.4968939999999999</v>
       </c>
       <c r="E241" t="n">
+        <v>27.41115646258503</v>
+      </c>
+      <c r="F241" t="n">
         <v>0.3677509427070618</v>
-      </c>
-      <c r="F241" t="n">
-        <v>4823.4375</v>
       </c>
       <c r="G241" t="inlineStr">
         <is>
@@ -6479,10 +6479,10 @@
         <v>0.062614</v>
       </c>
       <c r="E242" t="n">
+        <v>29.18748299319728</v>
+      </c>
+      <c r="F242" t="n">
         <v>0.3586937189102173</v>
-      </c>
-      <c r="F242" t="n">
-        <v>3014.6484375</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -6504,10 +6504,10 @@
         <v>0.309994</v>
       </c>
       <c r="E243" t="n">
+        <v>30.53424036281179</v>
+      </c>
+      <c r="F243" t="n">
         <v>0.5131331086158752</v>
-      </c>
-      <c r="F243" t="n">
-        <v>2950.048828125</v>
       </c>
       <c r="G243" t="inlineStr">
         <is>
@@ -6529,10 +6529,10 @@
         <v>-0.1925948</v>
       </c>
       <c r="E244" t="n">
+        <v>32.14802721088435</v>
+      </c>
+      <c r="F244" t="n">
         <v>0.3260004818439484</v>
-      </c>
-      <c r="F244" t="n">
-        <v>1507.32421875</v>
       </c>
       <c r="G244" t="inlineStr">
         <is>
@@ -6554,10 +6554,10 @@
         <v>0.006867899999999997</v>
       </c>
       <c r="E245" t="n">
+        <v>33.85469387755102</v>
+      </c>
+      <c r="F245" t="n">
         <v>0.3752983510494232</v>
-      </c>
-      <c r="F245" t="n">
-        <v>2217.919921875</v>
       </c>
       <c r="G245" t="inlineStr">
         <is>
@@ -6579,10 +6579,10 @@
         <v>0.0425392</v>
       </c>
       <c r="E246" t="n">
+        <v>36.501768707483</v>
+      </c>
+      <c r="F246" t="n">
         <v>0.3936578035354614</v>
-      </c>
-      <c r="F246" t="n">
-        <v>3100.78125</v>
       </c>
       <c r="G246" t="inlineStr">
         <is>
@@ -6604,10 +6604,10 @@
         <v>0.2529775</v>
       </c>
       <c r="E247" t="n">
+        <v>38.0691156462585</v>
+      </c>
+      <c r="F247" t="n">
         <v>0.3363303244113922</v>
-      </c>
-      <c r="F247" t="n">
-        <v>2282.51953125</v>
       </c>
       <c r="G247" t="inlineStr">
         <is>
@@ -6629,10 +6629,10 @@
         <v>0.474382</v>
       </c>
       <c r="E248" t="n">
+        <v>39.6712925170068</v>
+      </c>
+      <c r="F248" t="n">
         <v>0.381014496088028</v>
-      </c>
-      <c r="F248" t="n">
-        <v>2217.919921875</v>
       </c>
       <c r="G248" t="inlineStr">
         <is>
@@ -6654,10 +6654,10 @@
         <v>-0.0852769</v>
       </c>
       <c r="E249" t="n">
+        <v>41.08770975056689</v>
+      </c>
+      <c r="F249" t="n">
         <v>0.4283446967601776</v>
-      </c>
-      <c r="F249" t="n">
-        <v>2885.44921875</v>
       </c>
       <c r="G249" t="inlineStr">
         <is>
@@ -6679,10 +6679,10 @@
         <v>-0.3021668</v>
       </c>
       <c r="E250" t="n">
+        <v>43.68834467120181</v>
+      </c>
+      <c r="F250" t="n">
         <v>0.3728378117084503</v>
-      </c>
-      <c r="F250" t="n">
-        <v>2756.25</v>
       </c>
       <c r="G250" t="inlineStr">
         <is>
@@ -6704,10 +6704,10 @@
         <v>-0.2054215</v>
       </c>
       <c r="E251" t="n">
+        <v>45.44145124716553</v>
+      </c>
+      <c r="F251" t="n">
         <v>0.3864788115024567</v>
-      </c>
-      <c r="F251" t="n">
-        <v>2325.5859375</v>
       </c>
       <c r="G251" t="inlineStr">
         <is>
@@ -6729,10 +6729,10 @@
         <v>-0.469397</v>
       </c>
       <c r="E252" t="n">
+        <v>47.71700680272109</v>
+      </c>
+      <c r="F252" t="n">
         <v>0.3525626063346863</v>
-      </c>
-      <c r="F252" t="n">
-        <v>2605.517578125</v>
       </c>
       <c r="G252" t="inlineStr">
         <is>
@@ -6754,10 +6754,10 @@
         <v>-0.5889848</v>
       </c>
       <c r="E253" t="n">
+        <v>52.25650793650794</v>
+      </c>
+      <c r="F253" t="n">
         <v>0.4931949973106384</v>
-      </c>
-      <c r="F253" t="n">
-        <v>1399.658203125</v>
       </c>
       <c r="G253" t="inlineStr">
         <is>
@@ -6779,10 +6779,10 @@
         <v>0.1974002</v>
       </c>
       <c r="E254" t="n">
+        <v>5.479909297052155</v>
+      </c>
+      <c r="F254" t="n">
         <v>0.5518948435783386</v>
-      </c>
-      <c r="F254" t="n">
-        <v>1614.990234375</v>
       </c>
       <c r="G254" t="inlineStr">
         <is>
@@ -6804,10 +6804,10 @@
         <v>0.0247785</v>
       </c>
       <c r="E255" t="n">
+        <v>9.125442176870749</v>
+      </c>
+      <c r="F255" t="n">
         <v>0.4762373268604279</v>
-      </c>
-      <c r="F255" t="n">
-        <v>1485.791015625</v>
       </c>
       <c r="G255" t="inlineStr">
         <is>
@@ -6829,10 +6829,10 @@
         <v>-0.194585</v>
       </c>
       <c r="E256" t="n">
+        <v>11.76090702947846</v>
+      </c>
+      <c r="F256" t="n">
         <v>0.516711950302124</v>
-      </c>
-      <c r="F256" t="n">
-        <v>3079.248046875</v>
       </c>
       <c r="G256" t="inlineStr">
         <is>
@@ -6854,10 +6854,10 @@
         <v>-0.02853399999999999</v>
       </c>
       <c r="E257" t="n">
+        <v>14.04807256235828</v>
+      </c>
+      <c r="F257" t="n">
         <v>0.585009753704071</v>
-      </c>
-      <c r="F257" t="n">
-        <v>3552.978515625</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
@@ -6879,10 +6879,10 @@
         <v>0.1716195</v>
       </c>
       <c r="E258" t="n">
+        <v>14.53569160997732</v>
+      </c>
+      <c r="F258" t="n">
         <v>0.4687930941581726</v>
-      </c>
-      <c r="F258" t="n">
-        <v>2110.25390625</v>
       </c>
       <c r="G258" t="inlineStr">
         <is>
@@ -6904,10 +6904,10 @@
         <v>0.1680675</v>
       </c>
       <c r="E259" t="n">
+        <v>16.95056689342404</v>
+      </c>
+      <c r="F259" t="n">
         <v>0.5628640651702881</v>
-      </c>
-      <c r="F259" t="n">
-        <v>2993.115234375</v>
       </c>
       <c r="G259" t="inlineStr">
         <is>
@@ -6929,10 +6929,10 @@
         <v>0.1001665</v>
       </c>
       <c r="E260" t="n">
+        <v>20.67736961451247</v>
+      </c>
+      <c r="F260" t="n">
         <v>0.5198061466217041</v>
-      </c>
-      <c r="F260" t="n">
-        <v>3100.78125</v>
       </c>
       <c r="G260" t="inlineStr">
         <is>
@@ -6954,10 +6954,10 @@
         <v>-0.2907028</v>
       </c>
       <c r="E261" t="n">
+        <v>22.58140589569161</v>
+      </c>
+      <c r="F261" t="n">
         <v>0.5566231608390808</v>
-      </c>
-      <c r="F261" t="n">
-        <v>3079.248046875</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
@@ -6979,10 +6979,10 @@
         <v>0.1978245</v>
       </c>
       <c r="E262" t="n">
+        <v>24.46222222222222</v>
+      </c>
+      <c r="F262" t="n">
         <v>0.532808780670166</v>
-      </c>
-      <c r="F262" t="n">
-        <v>2906.982421875</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>
@@ -7004,10 +7004,10 @@
         <v>-0.2986295</v>
       </c>
       <c r="E263" t="n">
+        <v>25.78575963718821</v>
+      </c>
+      <c r="F263" t="n">
         <v>0.5040261149406433</v>
-      </c>
-      <c r="F263" t="n">
-        <v>3122.314453125</v>
       </c>
       <c r="G263" t="inlineStr">
         <is>
@@ -7029,10 +7029,10 @@
         <v>-0.134384</v>
       </c>
       <c r="E264" t="n">
+        <v>26.28498866213152</v>
+      </c>
+      <c r="F264" t="n">
         <v>0.2996820211410522</v>
-      </c>
-      <c r="F264" t="n">
-        <v>904.39453125</v>
       </c>
       <c r="G264" t="inlineStr">
         <is>
@@ -7054,10 +7054,10 @@
         <v>-0.0410635</v>
       </c>
       <c r="E265" t="n">
+        <v>29.5590022675737</v>
+      </c>
+      <c r="F265" t="n">
         <v>0.6519854068756104</v>
-      </c>
-      <c r="F265" t="n">
-        <v>3014.6484375</v>
       </c>
       <c r="G265" t="inlineStr">
         <is>
@@ -7079,10 +7079,10 @@
         <v>-0.179239</v>
       </c>
       <c r="E266" t="n">
+        <v>33.93596371882087</v>
+      </c>
+      <c r="F266" t="n">
         <v>0.6357070207595825</v>
-      </c>
-      <c r="F266" t="n">
-        <v>2993.115234375</v>
       </c>
       <c r="G266" t="inlineStr">
         <is>
@@ -7104,10 +7104,10 @@
         <v>0.06474850000000001</v>
       </c>
       <c r="E267" t="n">
+        <v>36.04897959183673</v>
+      </c>
+      <c r="F267" t="n">
         <v>0.5949224233627319</v>
-      </c>
-      <c r="F267" t="n">
-        <v>2971.58203125</v>
       </c>
       <c r="G267" t="inlineStr">
         <is>
@@ -7129,10 +7129,10 @@
         <v>0.349066</v>
       </c>
       <c r="E268" t="n">
+        <v>38.01106575963719</v>
+      </c>
+      <c r="F268" t="n">
         <v>0.5870410799980164</v>
-      </c>
-      <c r="F268" t="n">
-        <v>3122.314453125</v>
       </c>
       <c r="G268" t="inlineStr">
         <is>
@@ -7154,10 +7154,10 @@
         <v>-0.359791</v>
       </c>
       <c r="E269" t="n">
+        <v>38.95147392290249</v>
+      </c>
+      <c r="F269" t="n">
         <v>0.1923637390136719</v>
-      </c>
-      <c r="F269" t="n">
-        <v>1442.724609375</v>
       </c>
       <c r="G269" t="inlineStr">
         <is>
@@ -7179,10 +7179,10 @@
         <v>0.3113002</v>
       </c>
       <c r="E270" t="n">
+        <v>39.53197278911565</v>
+      </c>
+      <c r="F270" t="n">
         <v>0.5193952322006226</v>
-      </c>
-      <c r="F270" t="n">
-        <v>2906.982421875</v>
       </c>
       <c r="G270" t="inlineStr">
         <is>
@@ -7204,10 +7204,10 @@
         <v>0.335511</v>
       </c>
       <c r="E271" t="n">
+        <v>39.54358276643991</v>
+      </c>
+      <c r="F271" t="n">
         <v>0.4440512657165527</v>
-      </c>
-      <c r="F271" t="n">
-        <v>2088.720703125</v>
       </c>
       <c r="G271" t="inlineStr">
         <is>
@@ -7229,10 +7229,10 @@
         <v>-0.1085065</v>
       </c>
       <c r="E272" t="n">
+        <v>41.31990929705216</v>
+      </c>
+      <c r="F272" t="n">
         <v>0.5513631105422974</v>
-      </c>
-      <c r="F272" t="n">
-        <v>3014.6484375</v>
       </c>
       <c r="G272" t="inlineStr">
         <is>
@@ -7254,10 +7254,10 @@
         <v>0.394247</v>
       </c>
       <c r="E273" t="n">
+        <v>42.64344671201814</v>
+      </c>
+      <c r="F273" t="n">
         <v>0.5347734093666077</v>
-      </c>
-      <c r="F273" t="n">
-        <v>3208.447265625</v>
       </c>
       <c r="G273" t="inlineStr">
         <is>
@@ -7279,10 +7279,10 @@
         <v>-0.2650816</v>
       </c>
       <c r="E274" t="n">
+        <v>44.22240362811792</v>
+      </c>
+      <c r="F274" t="n">
         <v>0.5866594910621643</v>
-      </c>
-      <c r="F274" t="n">
-        <v>3079.248046875</v>
       </c>
       <c r="G274" t="inlineStr">
         <is>
@@ -7304,10 +7304,10 @@
         <v>0.437252</v>
       </c>
       <c r="E275" t="n">
+        <v>45.61560090702948</v>
+      </c>
+      <c r="F275" t="n">
         <v>0.4450651705265045</v>
-      </c>
-      <c r="F275" t="n">
-        <v>1873.388671875</v>
       </c>
       <c r="G275" t="inlineStr">
         <is>
@@ -7329,10 +7329,10 @@
         <v>-0.09645480000000001</v>
       </c>
       <c r="E276" t="n">
+        <v>47.49641723356009</v>
+      </c>
+      <c r="F276" t="n">
         <v>0.5460129976272583</v>
-      </c>
-      <c r="F276" t="n">
-        <v>3251.513671875</v>
       </c>
       <c r="G276" t="inlineStr">
         <is>
@@ -7354,10 +7354,10 @@
         <v>0.4793926</v>
       </c>
       <c r="E277" t="n">
+        <v>50.36408163265306</v>
+      </c>
+      <c r="F277" t="n">
         <v>0.498643159866333</v>
-      </c>
-      <c r="F277" t="n">
-        <v>2993.115234375</v>
       </c>
       <c r="G277" t="inlineStr">
         <is>
@@ -7379,10 +7379,10 @@
         <v>-0.07884200000000002</v>
       </c>
       <c r="E278" t="n">
+        <v>51.57151927437642</v>
+      </c>
+      <c r="F278" t="n">
         <v>0.2393325716257095</v>
-      </c>
-      <c r="F278" t="n">
-        <v>1012.060546875</v>
       </c>
       <c r="G278" t="inlineStr">
         <is>
@@ -7404,10 +7404,10 @@
         <v>0.05827700000000001</v>
       </c>
       <c r="E279" t="n">
+        <v>52.51192743764172</v>
+      </c>
+      <c r="F279" t="n">
         <v>0.4518710970878601</v>
-      </c>
-      <c r="F279" t="n">
-        <v>4651.171875</v>
       </c>
       <c r="G279" t="inlineStr">
         <is>
@@ -7429,10 +7429,10 @@
         <v>-0.3793238</v>
       </c>
       <c r="E280" t="n">
+        <v>54.11410430839003</v>
+      </c>
+      <c r="F280" t="n">
         <v>0.3910621106624603</v>
-      </c>
-      <c r="F280" t="n">
-        <v>2497.8515625</v>
       </c>
       <c r="G280" t="inlineStr">
         <is>
@@ -7454,10 +7454,10 @@
         <v>-0.04214149999999998</v>
       </c>
       <c r="E281" t="n">
+        <v>55.22866213151927</v>
+      </c>
+      <c r="F281" t="n">
         <v>0.4740928113460541</v>
-      </c>
-      <c r="F281" t="n">
-        <v>3725.244140625</v>
       </c>
       <c r="G281" t="inlineStr">
         <is>
@@ -7479,10 +7479,10 @@
         <v>0.241006</v>
       </c>
       <c r="E282" t="n">
+        <v>56.56380952380952</v>
+      </c>
+      <c r="F282" t="n">
         <v>0.518409252166748</v>
-      </c>
-      <c r="F282" t="n">
-        <v>3100.78125</v>
       </c>
       <c r="G282" t="inlineStr">
         <is>
@@ -7504,10 +7504,10 @@
         <v>-0.001470999999999993</v>
       </c>
       <c r="E283" t="n">
+        <v>58.10793650793651</v>
+      </c>
+      <c r="F283" t="n">
         <v>0.2294644415378571</v>
-      </c>
-      <c r="F283" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G283" t="inlineStr">
         <is>
@@ -7529,10 +7529,10 @@
         <v>0.357463</v>
       </c>
       <c r="E284" t="n">
+        <v>58.10793650793651</v>
+      </c>
+      <c r="F284" t="n">
         <v>0.6173584461212158</v>
-      </c>
-      <c r="F284" t="n">
-        <v>3294.580078125</v>
       </c>
       <c r="G284" t="inlineStr">
         <is>
@@ -7554,10 +7554,10 @@
         <v>-0.02092700000000002</v>
       </c>
       <c r="E285" t="n">
+        <v>0.01160997732426304</v>
+      </c>
+      <c r="F285" t="n">
         <v>0.4455823004245758</v>
-      </c>
-      <c r="F285" t="n">
-        <v>5211.03515625</v>
       </c>
       <c r="G285" t="inlineStr">
         <is>
@@ -7579,10 +7579,10 @@
         <v>0.207687</v>
       </c>
       <c r="E286" t="n">
+        <v>7.87156462585034</v>
+      </c>
+      <c r="F286" t="n">
         <v>0.4441018402576447</v>
-      </c>
-      <c r="F286" t="n">
-        <v>4629.638671875</v>
       </c>
       <c r="G286" t="inlineStr">
         <is>
@@ -7604,10 +7604,10 @@
         <v>-0.6464930000000001</v>
       </c>
       <c r="E287" t="n">
+        <v>10.49541950113379</v>
+      </c>
+      <c r="F287" t="n">
         <v>0.5523778200149536</v>
-      </c>
-      <c r="F287" t="n">
-        <v>1851.85546875</v>
       </c>
       <c r="G287" t="inlineStr">
         <is>
@@ -7629,10 +7629,10 @@
         <v>-0.104929</v>
       </c>
       <c r="E288" t="n">
+        <v>11.88861678004535</v>
+      </c>
+      <c r="F288" t="n">
         <v>0.3745413720607758</v>
-      </c>
-      <c r="F288" t="n">
-        <v>4737.3046875</v>
       </c>
       <c r="G288" t="inlineStr">
         <is>
@@ -7654,10 +7654,10 @@
         <v>-0.3734175</v>
       </c>
       <c r="E289" t="n">
+        <v>14.55891156462585</v>
+      </c>
+      <c r="F289" t="n">
         <v>0.3357652127742767</v>
-      </c>
-      <c r="F289" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G289" t="inlineStr">
         <is>
@@ -7679,10 +7679,10 @@
         <v>5.27684</v>
       </c>
       <c r="E290" t="n">
+        <v>14.57052154195011</v>
+      </c>
+      <c r="F290" t="n">
         <v>0.6234560608863831</v>
-      </c>
-      <c r="F290" t="n">
-        <v>2131.787109375</v>
       </c>
       <c r="G290" t="inlineStr">
         <is>
@@ -7704,10 +7704,10 @@
         <v>-0.01294259999999999</v>
       </c>
       <c r="E291" t="n">
+        <v>18.43664399092971</v>
+      </c>
+      <c r="F291" t="n">
         <v>0.428424745798111</v>
-      </c>
-      <c r="F291" t="n">
-        <v>2454.78515625</v>
       </c>
       <c r="G291" t="inlineStr">
         <is>
@@ -7729,10 +7729,10 @@
         <v>-0.05826199999999999</v>
       </c>
       <c r="E292" t="n">
+        <v>20.66575963718821</v>
+      </c>
+      <c r="F292" t="n">
         <v>0.4778189063072205</v>
-      </c>
-      <c r="F292" t="n">
-        <v>2368.65234375</v>
       </c>
       <c r="G292" t="inlineStr">
         <is>
@@ -7754,10 +7754,10 @@
         <v>-0.01409300000000005</v>
       </c>
       <c r="E293" t="n">
+        <v>21.39718820861678</v>
+      </c>
+      <c r="F293" t="n">
         <v>0.3147821128368378</v>
-      </c>
-      <c r="F293" t="n">
-        <v>4457.373046875</v>
       </c>
       <c r="G293" t="inlineStr">
         <is>
@@ -7779,10 +7779,10 @@
         <v>0.518972</v>
       </c>
       <c r="E294" t="n">
+        <v>27.2021768707483</v>
+      </c>
+      <c r="F294" t="n">
         <v>0.3000274002552032</v>
-      </c>
-      <c r="F294" t="n">
-        <v>5534.033203125</v>
       </c>
       <c r="G294" t="inlineStr">
         <is>
@@ -7804,10 +7804,10 @@
         <v>0.0005010000000000014</v>
       </c>
       <c r="E295" t="n">
+        <v>29.70993197278911</v>
+      </c>
+      <c r="F295" t="n">
         <v>0.5231661200523376</v>
-      </c>
-      <c r="F295" t="n">
-        <v>2519.384765625</v>
       </c>
       <c r="G295" t="inlineStr">
         <is>
@@ -7829,10 +7829,10 @@
         <v>-0.9926969999999999</v>
       </c>
       <c r="E296" t="n">
+        <v>30.39492063492063</v>
+      </c>
+      <c r="F296" t="n">
         <v>0.1655763536691666</v>
-      </c>
-      <c r="F296" t="n">
-        <v>839.794921875</v>
       </c>
       <c r="G296" t="inlineStr">
         <is>
@@ -7854,10 +7854,10 @@
         <v>-0.081201</v>
       </c>
       <c r="E297" t="n">
+        <v>32.49632653061224</v>
+      </c>
+      <c r="F297" t="n">
         <v>0.5504520535469055</v>
-      </c>
-      <c r="F297" t="n">
-        <v>2110.25390625</v>
       </c>
       <c r="G297" t="inlineStr">
         <is>
@@ -7879,10 +7879,10 @@
         <v>0.0518135</v>
       </c>
       <c r="E298" t="n">
+        <v>32.90267573696145</v>
+      </c>
+      <c r="F298" t="n">
         <v>0.3902859687805176</v>
-      </c>
-      <c r="F298" t="n">
-        <v>5792.431640625</v>
       </c>
       <c r="G298" t="inlineStr">
         <is>
@@ -7904,10 +7904,10 @@
         <v>0.07470900000000001</v>
       </c>
       <c r="E299" t="n">
+        <v>38.66122448979592</v>
+      </c>
+      <c r="F299" t="n">
         <v>0.398851066827774</v>
-      </c>
-      <c r="F299" t="n">
-        <v>4091.30859375</v>
       </c>
       <c r="G299" t="inlineStr">
         <is>
@@ -7929,10 +7929,10 @@
         <v>0.0261848</v>
       </c>
       <c r="E300" t="n">
+        <v>56.21551020408163</v>
+      </c>
+      <c r="F300" t="n">
         <v>0.4356667101383209</v>
-      </c>
-      <c r="F300" t="n">
-        <v>796.728515625</v>
       </c>
       <c r="G300" t="inlineStr">
         <is>
@@ -7954,10 +7954,10 @@
         <v>0.7448790000000001</v>
       </c>
       <c r="E301" t="n">
+        <v>0.09287981859410431</v>
+      </c>
+      <c r="F301" t="n">
         <v>0.2779751121997833</v>
-      </c>
-      <c r="F301" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G301" t="inlineStr">
         <is>
@@ -7979,10 +7979,10 @@
         <v>0.819006</v>
       </c>
       <c r="E302" t="n">
+        <v>2.948934240362812</v>
+      </c>
+      <c r="F302" t="n">
         <v>0.3085907995700836</v>
-      </c>
-      <c r="F302" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G302" t="inlineStr">
         <is>
@@ -8004,10 +8004,10 @@
         <v>0.190339</v>
       </c>
       <c r="E303" t="n">
+        <v>3.262403628117914</v>
+      </c>
+      <c r="F303" t="n">
         <v>0.5519975423812866</v>
-      </c>
-      <c r="F303" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G303" t="inlineStr">
         <is>
@@ -8029,10 +8029,10 @@
         <v>0.4186284</v>
       </c>
       <c r="E304" t="n">
+        <v>6.385487528344671</v>
+      </c>
+      <c r="F304" t="n">
         <v>0.3238067328929901</v>
-      </c>
-      <c r="F304" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G304" t="inlineStr">
         <is>
@@ -8054,10 +8054,10 @@
         <v>-0.003697000000000013</v>
       </c>
       <c r="E305" t="n">
+        <v>9.404081632653062</v>
+      </c>
+      <c r="F305" t="n">
         <v>0.2308726161718369</v>
-      </c>
-      <c r="F305" t="n">
-        <v>689.0625</v>
       </c>
       <c r="G305" t="inlineStr">
         <is>
@@ -8079,10 +8079,10 @@
         <v>0.01480479999999998</v>
       </c>
       <c r="E306" t="n">
+        <v>12.1556462585034</v>
+      </c>
+      <c r="F306" t="n">
         <v>0.2862644493579865</v>
-      </c>
-      <c r="F306" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G306" t="inlineStr">
         <is>
@@ -8104,10 +8104,10 @@
         <v>-0.471456</v>
       </c>
       <c r="E307" t="n">
+        <v>15.66185941043084</v>
+      </c>
+      <c r="F307" t="n">
         <v>0.3144614696502686</v>
-      </c>
-      <c r="F307" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G307" t="inlineStr">
         <is>
@@ -8129,10 +8129,10 @@
         <v>-0.566244</v>
       </c>
       <c r="E308" t="n">
+        <v>18.90104308390023</v>
+      </c>
+      <c r="F308" t="n">
         <v>0.2780390381813049</v>
-      </c>
-      <c r="F308" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G308" t="inlineStr">
         <is>
@@ -8154,10 +8154,10 @@
         <v>-0.6696435000000001</v>
       </c>
       <c r="E309" t="n">
+        <v>22.6162358276644</v>
+      </c>
+      <c r="F309" t="n">
         <v>0.2857031226158142</v>
-      </c>
-      <c r="F309" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G309" t="inlineStr">
         <is>
@@ -8179,10 +8179,10 @@
         <v>0.544061</v>
       </c>
       <c r="E310" t="n">
+        <v>25.51873015873016</v>
+      </c>
+      <c r="F310" t="n">
         <v>0.4109894931316376</v>
-      </c>
-      <c r="F310" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G310" t="inlineStr">
         <is>
@@ -8204,10 +8204,10 @@
         <v>-0.07789200000000002</v>
       </c>
       <c r="E311" t="n">
+        <v>30.278820861678</v>
+      </c>
+      <c r="F311" t="n">
         <v>0.3097386956214905</v>
-      </c>
-      <c r="F311" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G311" t="inlineStr">
         <is>
@@ -8229,10 +8229,10 @@
         <v>-0.03646500000000004</v>
       </c>
       <c r="E312" t="n">
+        <v>1.439637188208617</v>
+      </c>
+      <c r="F312" t="n">
         <v>0.347942590713501</v>
-      </c>
-      <c r="F312" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G312" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         <v>-0.007914000000000032</v>
       </c>
       <c r="E313" t="n">
+        <v>4.330521541950113</v>
+      </c>
+      <c r="F313" t="n">
         <v>0.3026096522808075</v>
-      </c>
-      <c r="F313" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G313" t="inlineStr">
         <is>
@@ -8279,10 +8279,10 @@
         <v>-0.1517585</v>
       </c>
       <c r="E314" t="n">
+        <v>6.942766439909297</v>
+      </c>
+      <c r="F314" t="n">
         <v>0.325267881155014</v>
-      </c>
-      <c r="F314" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G314" t="inlineStr">
         <is>
@@ -8304,10 +8304,10 @@
         <v>-1.086493</v>
       </c>
       <c r="E315" t="n">
+        <v>9.914920634920636</v>
+      </c>
+      <c r="F315" t="n">
         <v>0.3674872517585754</v>
-      </c>
-      <c r="F315" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G315" t="inlineStr">
         <is>
@@ -8329,10 +8329,10 @@
         <v>0.6160780000000001</v>
       </c>
       <c r="E316" t="n">
+        <v>13.5372335600907</v>
+      </c>
+      <c r="F316" t="n">
         <v>0.3199492394924164</v>
-      </c>
-      <c r="F316" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G316" t="inlineStr">
         <is>
@@ -8354,10 +8354,10 @@
         <v>-0.06011999999999999</v>
       </c>
       <c r="E317" t="n">
+        <v>16.31201814058957</v>
+      </c>
+      <c r="F317" t="n">
         <v>0.279223769903183</v>
-      </c>
-      <c r="F317" t="n">
-        <v>581.396484375</v>
       </c>
       <c r="G317" t="inlineStr">
         <is>
@@ -8379,10 +8379,10 @@
         <v>0.323619</v>
       </c>
       <c r="E318" t="n">
+        <v>19.23773242630385</v>
+      </c>
+      <c r="F318" t="n">
         <v>0.3571340441703796</v>
-      </c>
-      <c r="F318" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G318" t="inlineStr">
         <is>
@@ -8404,10 +8404,10 @@
         <v>0.302747</v>
       </c>
       <c r="E319" t="n">
+        <v>22.41886621315193</v>
+      </c>
+      <c r="F319" t="n">
         <v>0.3036279380321503</v>
-      </c>
-      <c r="F319" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G319" t="inlineStr">
         <is>
@@ -8429,10 +8429,10 @@
         <v>-0.141752</v>
       </c>
       <c r="E320" t="n">
+        <v>25.95990929705215</v>
+      </c>
+      <c r="F320" t="n">
         <v>0.2828925251960754</v>
-      </c>
-      <c r="F320" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G320" t="inlineStr">
         <is>
@@ -8454,10 +8454,10 @@
         <v>0.113794</v>
       </c>
       <c r="E321" t="n">
+        <v>28.57215419501134</v>
+      </c>
+      <c r="F321" t="n">
         <v>0.3461067080497742</v>
-      </c>
-      <c r="F321" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G321" t="inlineStr">
         <is>
@@ -8479,10 +8479,10 @@
         <v>0.446461</v>
       </c>
       <c r="E322" t="n">
+        <v>32.03192743764173</v>
+      </c>
+      <c r="F322" t="n">
         <v>0.3026132583618164</v>
-      </c>
-      <c r="F322" t="n">
-        <v>538.330078125</v>
       </c>
       <c r="G322" t="inlineStr">
         <is>
@@ -8504,10 +8504,10 @@
         <v>0.778385</v>
       </c>
       <c r="E323" t="n">
+        <v>34.1449433106576</v>
+      </c>
+      <c r="F323" t="n">
         <v>0.4492773413658142</v>
-      </c>
-      <c r="F323" t="n">
-        <v>279.931640625</v>
       </c>
       <c r="G323" t="inlineStr">
         <is>
@@ -8529,10 +8529,10 @@
         <v>0.3938574</v>
       </c>
       <c r="E324" t="n">
+        <v>35.398820861678</v>
+      </c>
+      <c r="F324" t="n">
         <v>0.2971603274345398</v>
-      </c>
-      <c r="F324" t="n">
-        <v>559.86328125</v>
       </c>
       <c r="G324" t="inlineStr">
         <is>
@@ -8554,10 +8554,10 @@
         <v>0.1304285</v>
       </c>
       <c r="E325" t="n">
+        <v>38.04589569160998</v>
+      </c>
+      <c r="F325" t="n">
         <v>0.3888822793960571</v>
-      </c>
-      <c r="F325" t="n">
-        <v>495.263671875</v>
       </c>
       <c r="G325" t="inlineStr">
         <is>
@@ -8579,10 +8579,10 @@
         <v>-0.08117880000000001</v>
       </c>
       <c r="E326" t="n">
+        <v>41.87718820861678</v>
+      </c>
+      <c r="F326" t="n">
         <v>0.3490855097770691</v>
-      </c>
-      <c r="F326" t="n">
-        <v>452.197265625</v>
       </c>
       <c r="G326" t="inlineStr">
         <is>
@@ -8604,10 +8604,10 @@
         <v>-0.421693</v>
       </c>
       <c r="E327" t="n">
+        <v>44.59392290249433</v>
+      </c>
+      <c r="F327" t="n">
         <v>0.3239328861236572</v>
-      </c>
-      <c r="F327" t="n">
-        <v>473.73046875</v>
       </c>
       <c r="G327" t="inlineStr">
         <is>
@@ -8629,10 +8629,10 @@
         <v>-0.119105</v>
       </c>
       <c r="E328" t="n">
+        <v>46.78820861678005</v>
+      </c>
+      <c r="F328" t="n">
         <v>0.3749678730964661</v>
-      </c>
-      <c r="F328" t="n">
-        <v>301.46484375</v>
       </c>
       <c r="G328" t="inlineStr">
         <is>
@@ -8654,10 +8654,10 @@
         <v>-1.099002</v>
       </c>
       <c r="E329" t="n">
+        <v>49.01732426303855</v>
+      </c>
+      <c r="F329" t="n">
         <v>0.3135745525360107</v>
-      </c>
-      <c r="F329" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G329" t="inlineStr">
         <is>
@@ -8679,10 +8679,10 @@
         <v>0.2436524</v>
       </c>
       <c r="E330" t="n">
+        <v>52.03591836734694</v>
+      </c>
+      <c r="F330" t="n">
         <v>0.3206560015678406</v>
-      </c>
-      <c r="F330" t="n">
-        <v>516.796875</v>
       </c>
       <c r="G330" t="inlineStr">
         <is>

</xml_diff>